<commit_message>
adding new 2024 data
</commit_message>
<xml_diff>
--- a/data/2024Perley/qPCR/APC0264 Final qPCR Results_20-Nov-24.xlsx
+++ b/data/2024Perley/qPCR/APC0264 Final qPCR Results_20-Nov-24.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Science\CESD\ABL\Project Files\eDNA\APC0264\qPCR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9992D58D-BC00-46D0-9270-576962E183BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{9992D58D-BC00-46D0-9270-576962E183BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56A2BEEF-2581-44A3-BBE2-8D9D7BA993D8}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4A1A4D67-35D0-4F70-9268-641233523700}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4A1A4D67-35D0-4F70-9268-641233523700}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="4" r:id="rId1"/>
     <sheet name="Detailed Results" sheetId="1" r:id="rId2"/>
     <sheet name="Decision Tree" sheetId="5" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Detailed Results'!$A$1:$BC$125</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1866,6 +1869,63 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1878,62 +1938,59 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1956,64 +2013,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2387,8 +2390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB15AE7B-D81D-4A7B-8942-933F37740672}">
   <dimension ref="A1:U127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3:L5"/>
+    <sheetView topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="L105" activeCellId="8" sqref="L9:L11 L13:L27 L33:L50 L57:L65 L68:L73 L75:L89 L91:L96 L99:L103 L105:L109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2408,11 +2411,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" thickBot="1">
-      <c r="L1" s="166" t="s">
+      <c r="L1" s="146" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="167"/>
-      <c r="N1" s="168"/>
+      <c r="M1" s="147"/>
+      <c r="N1" s="148"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickBot="1">
       <c r="A2" s="94" t="s">
@@ -2499,10 +2502,10 @@
       <c r="K3" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="149" t="s">
+      <c r="L3" s="168" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="156" t="s">
+      <c r="M3" s="159" t="s">
         <v>23</v>
       </c>
       <c r="N3" s="161" t="s">
@@ -2543,8 +2546,8 @@
       <c r="K4" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="150"/>
-      <c r="M4" s="156"/>
+      <c r="L4" s="156"/>
+      <c r="M4" s="159"/>
       <c r="N4" s="153"/>
     </row>
     <row r="5" spans="1:21">
@@ -2581,8 +2584,8 @@
       <c r="K5" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="151"/>
-      <c r="M5" s="157"/>
+      <c r="L5" s="157"/>
+      <c r="M5" s="160"/>
       <c r="N5" s="154"/>
     </row>
     <row r="6" spans="1:21">
@@ -2622,7 +2625,7 @@
       <c r="L6" s="152" t="s">
         <v>24</v>
       </c>
-      <c r="M6" s="155" t="s">
+      <c r="M6" s="158" t="s">
         <v>23</v>
       </c>
       <c r="N6" s="152" t="s">
@@ -2664,7 +2667,7 @@
         <v>21</v>
       </c>
       <c r="L7" s="153"/>
-      <c r="M7" s="156"/>
+      <c r="M7" s="159"/>
       <c r="N7" s="153"/>
     </row>
     <row r="8" spans="1:21">
@@ -2702,7 +2705,7 @@
         <v>21</v>
       </c>
       <c r="L8" s="154"/>
-      <c r="M8" s="157"/>
+      <c r="M8" s="160"/>
       <c r="N8" s="154"/>
     </row>
     <row r="9" spans="1:21">
@@ -2739,10 +2742,10 @@
       <c r="K9" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L9" s="146" t="s">
+      <c r="L9" s="165" t="s">
         <v>23</v>
       </c>
-      <c r="M9" s="155" t="s">
+      <c r="M9" s="158" t="s">
         <v>23</v>
       </c>
       <c r="N9" s="152" t="s">
@@ -2783,8 +2786,8 @@
       <c r="K10" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="147"/>
-      <c r="M10" s="156"/>
+      <c r="L10" s="166"/>
+      <c r="M10" s="159"/>
       <c r="N10" s="153"/>
     </row>
     <row r="11" spans="1:21">
@@ -2821,8 +2824,8 @@
       <c r="K11" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="L11" s="148"/>
-      <c r="M11" s="157"/>
+      <c r="L11" s="167"/>
+      <c r="M11" s="160"/>
       <c r="N11" s="154"/>
     </row>
     <row r="12" spans="1:21">
@@ -2903,10 +2906,10 @@
       <c r="K13" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L13" s="146" t="s">
+      <c r="L13" s="165" t="s">
         <v>23</v>
       </c>
-      <c r="M13" s="155" t="s">
+      <c r="M13" s="158" t="s">
         <v>23</v>
       </c>
       <c r="N13" s="152" t="s">
@@ -2947,8 +2950,8 @@
       <c r="K14" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L14" s="147"/>
-      <c r="M14" s="156"/>
+      <c r="L14" s="166"/>
+      <c r="M14" s="159"/>
       <c r="N14" s="153"/>
     </row>
     <row r="15" spans="1:21">
@@ -2985,8 +2988,8 @@
       <c r="K15" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="L15" s="148"/>
-      <c r="M15" s="157"/>
+      <c r="L15" s="167"/>
+      <c r="M15" s="160"/>
       <c r="N15" s="154"/>
     </row>
     <row r="16" spans="1:21">
@@ -3023,10 +3026,10 @@
       <c r="K16" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L16" s="146" t="s">
+      <c r="L16" s="165" t="s">
         <v>23</v>
       </c>
-      <c r="M16" s="155" t="s">
+      <c r="M16" s="158" t="s">
         <v>23</v>
       </c>
       <c r="N16" s="152" t="s">
@@ -3067,8 +3070,8 @@
       <c r="K17" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L17" s="147"/>
-      <c r="M17" s="156"/>
+      <c r="L17" s="166"/>
+      <c r="M17" s="159"/>
       <c r="N17" s="153"/>
     </row>
     <row r="18" spans="1:15">
@@ -3105,8 +3108,8 @@
       <c r="K18" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="L18" s="148"/>
-      <c r="M18" s="157"/>
+      <c r="L18" s="167"/>
+      <c r="M18" s="160"/>
       <c r="N18" s="154"/>
     </row>
     <row r="19" spans="1:15">
@@ -3143,10 +3146,10 @@
       <c r="K19" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L19" s="146" t="s">
+      <c r="L19" s="165" t="s">
         <v>23</v>
       </c>
-      <c r="M19" s="155" t="s">
+      <c r="M19" s="158" t="s">
         <v>23</v>
       </c>
       <c r="N19" s="152" t="s">
@@ -3187,8 +3190,8 @@
       <c r="K20" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L20" s="147"/>
-      <c r="M20" s="156"/>
+      <c r="L20" s="166"/>
+      <c r="M20" s="159"/>
       <c r="N20" s="153"/>
     </row>
     <row r="21" spans="1:15">
@@ -3225,8 +3228,8 @@
       <c r="K21" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="L21" s="148"/>
-      <c r="M21" s="157"/>
+      <c r="L21" s="167"/>
+      <c r="M21" s="160"/>
       <c r="N21" s="154"/>
     </row>
     <row r="22" spans="1:15">
@@ -3263,10 +3266,10 @@
       <c r="K22" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L22" s="146" t="s">
+      <c r="L22" s="165" t="s">
         <v>23</v>
       </c>
-      <c r="M22" s="155" t="s">
+      <c r="M22" s="158" t="s">
         <v>23</v>
       </c>
       <c r="N22" s="152" t="s">
@@ -3307,8 +3310,8 @@
       <c r="K23" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L23" s="147"/>
-      <c r="M23" s="156"/>
+      <c r="L23" s="166"/>
+      <c r="M23" s="159"/>
       <c r="N23" s="153"/>
     </row>
     <row r="24" spans="1:15">
@@ -3345,8 +3348,8 @@
       <c r="K24" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="L24" s="148"/>
-      <c r="M24" s="157"/>
+      <c r="L24" s="167"/>
+      <c r="M24" s="160"/>
       <c r="N24" s="154"/>
     </row>
     <row r="25" spans="1:15">
@@ -3383,10 +3386,10 @@
       <c r="K25" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L25" s="146" t="s">
+      <c r="L25" s="165" t="s">
         <v>23</v>
       </c>
-      <c r="M25" s="155" t="s">
+      <c r="M25" s="158" t="s">
         <v>23</v>
       </c>
       <c r="N25" s="152" t="s">
@@ -3427,8 +3430,8 @@
       <c r="K26" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L26" s="147"/>
-      <c r="M26" s="156"/>
+      <c r="L26" s="166"/>
+      <c r="M26" s="159"/>
       <c r="N26" s="153"/>
     </row>
     <row r="27" spans="1:15">
@@ -3465,8 +3468,8 @@
       <c r="K27" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="L27" s="148"/>
-      <c r="M27" s="157"/>
+      <c r="L27" s="167"/>
+      <c r="M27" s="160"/>
       <c r="N27" s="154"/>
     </row>
     <row r="28" spans="1:15">
@@ -3550,10 +3553,10 @@
       <c r="L29" s="152" t="s">
         <v>24</v>
       </c>
-      <c r="M29" s="158" t="s">
-        <v>24</v>
-      </c>
-      <c r="N29" s="162" t="s">
+      <c r="M29" s="162" t="s">
+        <v>24</v>
+      </c>
+      <c r="N29" s="149" t="s">
         <v>22</v>
       </c>
     </row>
@@ -3592,8 +3595,8 @@
         <v>21</v>
       </c>
       <c r="L30" s="153"/>
-      <c r="M30" s="159"/>
-      <c r="N30" s="163"/>
+      <c r="M30" s="163"/>
+      <c r="N30" s="150"/>
     </row>
     <row r="31" spans="1:15">
       <c r="A31" s="74">
@@ -3630,8 +3633,8 @@
         <v>21</v>
       </c>
       <c r="L31" s="154"/>
-      <c r="M31" s="160"/>
-      <c r="N31" s="164"/>
+      <c r="M31" s="164"/>
+      <c r="N31" s="151"/>
     </row>
     <row r="32" spans="1:15">
       <c r="A32" s="86">
@@ -3714,10 +3717,10 @@
       <c r="K33" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L33" s="146" t="s">
+      <c r="L33" s="165" t="s">
         <v>23</v>
       </c>
-      <c r="M33" s="155" t="s">
+      <c r="M33" s="158" t="s">
         <v>23</v>
       </c>
       <c r="N33" s="152" t="s">
@@ -3758,8 +3761,8 @@
       <c r="K34" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L34" s="147"/>
-      <c r="M34" s="156"/>
+      <c r="L34" s="166"/>
+      <c r="M34" s="159"/>
       <c r="N34" s="153"/>
     </row>
     <row r="35" spans="1:14">
@@ -3796,8 +3799,8 @@
       <c r="K35" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="L35" s="148"/>
-      <c r="M35" s="157"/>
+      <c r="L35" s="167"/>
+      <c r="M35" s="160"/>
       <c r="N35" s="154"/>
     </row>
     <row r="36" spans="1:14">
@@ -3834,13 +3837,13 @@
       <c r="K36" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L36" s="146" t="s">
+      <c r="L36" s="165" t="s">
         <v>23</v>
       </c>
-      <c r="M36" s="155" t="s">
+      <c r="M36" s="158" t="s">
         <v>23</v>
       </c>
-      <c r="N36" s="162" t="s">
+      <c r="N36" s="149" t="s">
         <v>22</v>
       </c>
     </row>
@@ -3878,9 +3881,9 @@
       <c r="K37" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L37" s="147"/>
-      <c r="M37" s="156"/>
-      <c r="N37" s="163"/>
+      <c r="L37" s="166"/>
+      <c r="M37" s="159"/>
+      <c r="N37" s="150"/>
     </row>
     <row r="38" spans="1:14">
       <c r="A38" s="76">
@@ -3916,9 +3919,9 @@
       <c r="K38" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="L38" s="148"/>
-      <c r="M38" s="157"/>
-      <c r="N38" s="164"/>
+      <c r="L38" s="167"/>
+      <c r="M38" s="160"/>
+      <c r="N38" s="151"/>
     </row>
     <row r="39" spans="1:14">
       <c r="A39" s="66">
@@ -3954,13 +3957,13 @@
       <c r="K39" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L39" s="146" t="s">
+      <c r="L39" s="165" t="s">
         <v>23</v>
       </c>
-      <c r="M39" s="155" t="s">
+      <c r="M39" s="158" t="s">
         <v>23</v>
       </c>
-      <c r="N39" s="165" t="s">
+      <c r="N39" s="155" t="s">
         <v>22</v>
       </c>
     </row>
@@ -3998,9 +4001,9 @@
       <c r="K40" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L40" s="147"/>
-      <c r="M40" s="156"/>
-      <c r="N40" s="150"/>
+      <c r="L40" s="166"/>
+      <c r="M40" s="159"/>
+      <c r="N40" s="156"/>
     </row>
     <row r="41" spans="1:14">
       <c r="A41" s="76">
@@ -4036,9 +4039,9 @@
       <c r="K41" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="L41" s="148"/>
-      <c r="M41" s="157"/>
-      <c r="N41" s="151"/>
+      <c r="L41" s="167"/>
+      <c r="M41" s="160"/>
+      <c r="N41" s="157"/>
     </row>
     <row r="42" spans="1:14">
       <c r="A42" s="66">
@@ -4074,10 +4077,10 @@
       <c r="K42" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L42" s="146" t="s">
+      <c r="L42" s="165" t="s">
         <v>23</v>
       </c>
-      <c r="M42" s="155" t="s">
+      <c r="M42" s="158" t="s">
         <v>23</v>
       </c>
       <c r="N42" s="152" t="s">
@@ -4118,8 +4121,8 @@
       <c r="K43" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L43" s="147"/>
-      <c r="M43" s="156"/>
+      <c r="L43" s="166"/>
+      <c r="M43" s="159"/>
       <c r="N43" s="153"/>
     </row>
     <row r="44" spans="1:14">
@@ -4156,8 +4159,8 @@
       <c r="K44" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="L44" s="148"/>
-      <c r="M44" s="157"/>
+      <c r="L44" s="167"/>
+      <c r="M44" s="160"/>
       <c r="N44" s="154"/>
     </row>
     <row r="45" spans="1:14">
@@ -4194,10 +4197,10 @@
       <c r="K45" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L45" s="146" t="s">
+      <c r="L45" s="165" t="s">
         <v>23</v>
       </c>
-      <c r="M45" s="155" t="s">
+      <c r="M45" s="158" t="s">
         <v>23</v>
       </c>
       <c r="N45" s="152" t="s">
@@ -4238,8 +4241,8 @@
       <c r="K46" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L46" s="147"/>
-      <c r="M46" s="156"/>
+      <c r="L46" s="166"/>
+      <c r="M46" s="159"/>
       <c r="N46" s="153"/>
     </row>
     <row r="47" spans="1:14">
@@ -4276,8 +4279,8 @@
       <c r="K47" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="L47" s="148"/>
-      <c r="M47" s="157"/>
+      <c r="L47" s="167"/>
+      <c r="M47" s="160"/>
       <c r="N47" s="154"/>
     </row>
     <row r="48" spans="1:14">
@@ -4314,10 +4317,10 @@
       <c r="K48" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L48" s="146" t="s">
+      <c r="L48" s="165" t="s">
         <v>23</v>
       </c>
-      <c r="M48" s="155" t="s">
+      <c r="M48" s="158" t="s">
         <v>23</v>
       </c>
       <c r="N48" s="152" t="s">
@@ -4358,8 +4361,8 @@
       <c r="K49" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L49" s="147"/>
-      <c r="M49" s="156"/>
+      <c r="L49" s="166"/>
+      <c r="M49" s="159"/>
       <c r="N49" s="153"/>
     </row>
     <row r="50" spans="1:14">
@@ -4396,8 +4399,8 @@
       <c r="K50" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="L50" s="148"/>
-      <c r="M50" s="157"/>
+      <c r="L50" s="167"/>
+      <c r="M50" s="160"/>
       <c r="N50" s="154"/>
     </row>
     <row r="51" spans="1:14">
@@ -4437,7 +4440,7 @@
       <c r="L51" s="152" t="s">
         <v>24</v>
       </c>
-      <c r="M51" s="158" t="s">
+      <c r="M51" s="162" t="s">
         <v>24</v>
       </c>
       <c r="N51" s="152" t="s">
@@ -4479,7 +4482,7 @@
         <v>21</v>
       </c>
       <c r="L52" s="153"/>
-      <c r="M52" s="159"/>
+      <c r="M52" s="163"/>
       <c r="N52" s="153"/>
     </row>
     <row r="53" spans="1:14">
@@ -4517,7 +4520,7 @@
         <v>21</v>
       </c>
       <c r="L53" s="154"/>
-      <c r="M53" s="160"/>
+      <c r="M53" s="164"/>
       <c r="N53" s="154"/>
     </row>
     <row r="54" spans="1:14">
@@ -4557,7 +4560,7 @@
       <c r="L54" s="152" t="s">
         <v>24</v>
       </c>
-      <c r="M54" s="155" t="s">
+      <c r="M54" s="158" t="s">
         <v>23</v>
       </c>
       <c r="N54" s="152" t="s">
@@ -4599,7 +4602,7 @@
         <v>21</v>
       </c>
       <c r="L55" s="153"/>
-      <c r="M55" s="156"/>
+      <c r="M55" s="159"/>
       <c r="N55" s="153"/>
     </row>
     <row r="56" spans="1:14">
@@ -4637,7 +4640,7 @@
         <v>21</v>
       </c>
       <c r="L56" s="154"/>
-      <c r="M56" s="157"/>
+      <c r="M56" s="160"/>
       <c r="N56" s="154"/>
     </row>
     <row r="57" spans="1:14">
@@ -4674,10 +4677,10 @@
       <c r="K57" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L57" s="146" t="s">
+      <c r="L57" s="165" t="s">
         <v>23</v>
       </c>
-      <c r="M57" s="155" t="s">
+      <c r="M57" s="158" t="s">
         <v>23</v>
       </c>
       <c r="N57" s="152" t="s">
@@ -4718,8 +4721,8 @@
       <c r="K58" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L58" s="147"/>
-      <c r="M58" s="156"/>
+      <c r="L58" s="166"/>
+      <c r="M58" s="159"/>
       <c r="N58" s="153"/>
     </row>
     <row r="59" spans="1:14">
@@ -4756,8 +4759,8 @@
       <c r="K59" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="L59" s="148"/>
-      <c r="M59" s="157"/>
+      <c r="L59" s="167"/>
+      <c r="M59" s="160"/>
       <c r="N59" s="154"/>
     </row>
     <row r="60" spans="1:14">
@@ -4794,13 +4797,13 @@
       <c r="K60" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L60" s="146" t="s">
+      <c r="L60" s="165" t="s">
         <v>23</v>
       </c>
-      <c r="M60" s="155" t="s">
+      <c r="M60" s="158" t="s">
         <v>23</v>
       </c>
-      <c r="N60" s="162" t="s">
+      <c r="N60" s="149" t="s">
         <v>22</v>
       </c>
     </row>
@@ -4838,9 +4841,9 @@
       <c r="K61" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L61" s="147"/>
-      <c r="M61" s="156"/>
-      <c r="N61" s="163"/>
+      <c r="L61" s="166"/>
+      <c r="M61" s="159"/>
+      <c r="N61" s="150"/>
     </row>
     <row r="62" spans="1:14">
       <c r="A62" s="76">
@@ -4876,9 +4879,9 @@
       <c r="K62" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="L62" s="148"/>
-      <c r="M62" s="157"/>
-      <c r="N62" s="164"/>
+      <c r="L62" s="167"/>
+      <c r="M62" s="160"/>
+      <c r="N62" s="151"/>
     </row>
     <row r="63" spans="1:14">
       <c r="A63" s="66">
@@ -4914,10 +4917,10 @@
       <c r="K63" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L63" s="146" t="s">
+      <c r="L63" s="165" t="s">
         <v>23</v>
       </c>
-      <c r="M63" s="155" t="s">
+      <c r="M63" s="158" t="s">
         <v>23</v>
       </c>
       <c r="N63" s="152" t="s">
@@ -4958,8 +4961,8 @@
       <c r="K64" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L64" s="147"/>
-      <c r="M64" s="156"/>
+      <c r="L64" s="166"/>
+      <c r="M64" s="159"/>
       <c r="N64" s="153"/>
     </row>
     <row r="65" spans="1:14">
@@ -4996,8 +4999,8 @@
       <c r="K65" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="L65" s="148"/>
-      <c r="M65" s="157"/>
+      <c r="L65" s="167"/>
+      <c r="M65" s="160"/>
       <c r="N65" s="154"/>
     </row>
     <row r="66" spans="1:14">
@@ -5122,10 +5125,10 @@
       <c r="K68" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L68" s="146" t="s">
+      <c r="L68" s="165" t="s">
         <v>23</v>
       </c>
-      <c r="M68" s="155" t="s">
+      <c r="M68" s="158" t="s">
         <v>23</v>
       </c>
       <c r="N68" s="152" t="s">
@@ -5166,8 +5169,8 @@
       <c r="K69" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L69" s="147"/>
-      <c r="M69" s="156"/>
+      <c r="L69" s="166"/>
+      <c r="M69" s="159"/>
       <c r="N69" s="153"/>
     </row>
     <row r="70" spans="1:14">
@@ -5204,8 +5207,8 @@
       <c r="K70" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="L70" s="148"/>
-      <c r="M70" s="157"/>
+      <c r="L70" s="167"/>
+      <c r="M70" s="160"/>
       <c r="N70" s="154"/>
     </row>
     <row r="71" spans="1:14">
@@ -5242,13 +5245,13 @@
       <c r="K71" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L71" s="146" t="s">
+      <c r="L71" s="165" t="s">
         <v>23</v>
       </c>
-      <c r="M71" s="155" t="s">
+      <c r="M71" s="158" t="s">
         <v>23</v>
       </c>
-      <c r="N71" s="165" t="s">
+      <c r="N71" s="155" t="s">
         <v>22</v>
       </c>
     </row>
@@ -5286,9 +5289,9 @@
       <c r="K72" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L72" s="147"/>
-      <c r="M72" s="156"/>
-      <c r="N72" s="150"/>
+      <c r="L72" s="166"/>
+      <c r="M72" s="159"/>
+      <c r="N72" s="156"/>
     </row>
     <row r="73" spans="1:14">
       <c r="A73" s="76">
@@ -5324,9 +5327,9 @@
       <c r="K73" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="L73" s="148"/>
-      <c r="M73" s="157"/>
-      <c r="N73" s="151"/>
+      <c r="L73" s="167"/>
+      <c r="M73" s="160"/>
+      <c r="N73" s="157"/>
     </row>
     <row r="74" spans="1:14">
       <c r="A74" s="76">
@@ -5406,10 +5409,10 @@
       <c r="K75" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L75" s="146" t="s">
+      <c r="L75" s="165" t="s">
         <v>23</v>
       </c>
-      <c r="M75" s="155" t="s">
+      <c r="M75" s="158" t="s">
         <v>23</v>
       </c>
       <c r="N75" s="152" t="s">
@@ -5450,8 +5453,8 @@
       <c r="K76" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L76" s="147"/>
-      <c r="M76" s="156"/>
+      <c r="L76" s="166"/>
+      <c r="M76" s="159"/>
       <c r="N76" s="153"/>
     </row>
     <row r="77" spans="1:14">
@@ -5488,8 +5491,8 @@
       <c r="K77" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="L77" s="148"/>
-      <c r="M77" s="157"/>
+      <c r="L77" s="167"/>
+      <c r="M77" s="160"/>
       <c r="N77" s="154"/>
     </row>
     <row r="78" spans="1:14">
@@ -5526,10 +5529,10 @@
       <c r="K78" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L78" s="146" t="s">
+      <c r="L78" s="165" t="s">
         <v>23</v>
       </c>
-      <c r="M78" s="155" t="s">
+      <c r="M78" s="158" t="s">
         <v>23</v>
       </c>
       <c r="N78" s="152" t="s">
@@ -5570,8 +5573,8 @@
       <c r="K79" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L79" s="147"/>
-      <c r="M79" s="156"/>
+      <c r="L79" s="166"/>
+      <c r="M79" s="159"/>
       <c r="N79" s="153"/>
     </row>
     <row r="80" spans="1:14">
@@ -5608,8 +5611,8 @@
       <c r="K80" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="L80" s="148"/>
-      <c r="M80" s="157"/>
+      <c r="L80" s="167"/>
+      <c r="M80" s="160"/>
       <c r="N80" s="154"/>
     </row>
     <row r="81" spans="1:14">
@@ -5646,10 +5649,10 @@
       <c r="K81" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L81" s="146" t="s">
+      <c r="L81" s="165" t="s">
         <v>23</v>
       </c>
-      <c r="M81" s="155" t="s">
+      <c r="M81" s="158" t="s">
         <v>23</v>
       </c>
       <c r="N81" s="152" t="s">
@@ -5690,8 +5693,8 @@
       <c r="K82" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L82" s="147"/>
-      <c r="M82" s="156"/>
+      <c r="L82" s="166"/>
+      <c r="M82" s="159"/>
       <c r="N82" s="153"/>
     </row>
     <row r="83" spans="1:14">
@@ -5728,8 +5731,8 @@
       <c r="K83" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="L83" s="148"/>
-      <c r="M83" s="157"/>
+      <c r="L83" s="167"/>
+      <c r="M83" s="160"/>
       <c r="N83" s="154"/>
     </row>
     <row r="84" spans="1:14">
@@ -5766,10 +5769,10 @@
       <c r="K84" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L84" s="146" t="s">
+      <c r="L84" s="165" t="s">
         <v>23</v>
       </c>
-      <c r="M84" s="155" t="s">
+      <c r="M84" s="158" t="s">
         <v>23</v>
       </c>
       <c r="N84" s="152" t="s">
@@ -5810,8 +5813,8 @@
       <c r="K85" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L85" s="147"/>
-      <c r="M85" s="156"/>
+      <c r="L85" s="166"/>
+      <c r="M85" s="159"/>
       <c r="N85" s="153"/>
     </row>
     <row r="86" spans="1:14">
@@ -5848,8 +5851,8 @@
       <c r="K86" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="L86" s="148"/>
-      <c r="M86" s="157"/>
+      <c r="L86" s="167"/>
+      <c r="M86" s="160"/>
       <c r="N86" s="154"/>
     </row>
     <row r="87" spans="1:14">
@@ -5886,10 +5889,10 @@
       <c r="K87" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L87" s="146" t="s">
+      <c r="L87" s="165" t="s">
         <v>23</v>
       </c>
-      <c r="M87" s="155" t="s">
+      <c r="M87" s="158" t="s">
         <v>23</v>
       </c>
       <c r="N87" s="152" t="s">
@@ -5930,8 +5933,8 @@
       <c r="K88" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L88" s="147"/>
-      <c r="M88" s="156"/>
+      <c r="L88" s="166"/>
+      <c r="M88" s="159"/>
       <c r="N88" s="153"/>
     </row>
     <row r="89" spans="1:14">
@@ -5968,8 +5971,8 @@
       <c r="K89" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="L89" s="148"/>
-      <c r="M89" s="157"/>
+      <c r="L89" s="167"/>
+      <c r="M89" s="160"/>
       <c r="N89" s="154"/>
     </row>
     <row r="90" spans="1:14">
@@ -6050,13 +6053,13 @@
       <c r="K91" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L91" s="146" t="s">
+      <c r="L91" s="165" t="s">
         <v>23</v>
       </c>
-      <c r="M91" s="155" t="s">
+      <c r="M91" s="158" t="s">
         <v>23</v>
       </c>
-      <c r="N91" s="162" t="s">
+      <c r="N91" s="149" t="s">
         <v>22</v>
       </c>
     </row>
@@ -6094,9 +6097,9 @@
       <c r="K92" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L92" s="147"/>
-      <c r="M92" s="156"/>
-      <c r="N92" s="163"/>
+      <c r="L92" s="166"/>
+      <c r="M92" s="159"/>
+      <c r="N92" s="150"/>
     </row>
     <row r="93" spans="1:14">
       <c r="A93" s="76">
@@ -6132,9 +6135,9 @@
       <c r="K93" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="L93" s="148"/>
-      <c r="M93" s="157"/>
-      <c r="N93" s="164"/>
+      <c r="L93" s="167"/>
+      <c r="M93" s="160"/>
+      <c r="N93" s="151"/>
     </row>
     <row r="94" spans="1:14">
       <c r="A94" s="66">
@@ -6170,10 +6173,10 @@
       <c r="K94" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L94" s="146" t="s">
+      <c r="L94" s="165" t="s">
         <v>23</v>
       </c>
-      <c r="M94" s="155" t="s">
+      <c r="M94" s="158" t="s">
         <v>23</v>
       </c>
       <c r="N94" s="152" t="s">
@@ -6214,8 +6217,8 @@
       <c r="K95" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L95" s="147"/>
-      <c r="M95" s="156"/>
+      <c r="L95" s="166"/>
+      <c r="M95" s="159"/>
       <c r="N95" s="153"/>
     </row>
     <row r="96" spans="1:14">
@@ -6252,8 +6255,8 @@
       <c r="K96" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="L96" s="148"/>
-      <c r="M96" s="157"/>
+      <c r="L96" s="167"/>
+      <c r="M96" s="160"/>
       <c r="N96" s="154"/>
     </row>
     <row r="97" spans="1:14">
@@ -6373,10 +6376,10 @@
       <c r="K99" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L99" s="146" t="s">
+      <c r="L99" s="165" t="s">
         <v>23</v>
       </c>
-      <c r="M99" s="155" t="s">
+      <c r="M99" s="158" t="s">
         <v>23</v>
       </c>
       <c r="N99" s="152" t="s">
@@ -6414,8 +6417,8 @@
       <c r="K100" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L100" s="147"/>
-      <c r="M100" s="156"/>
+      <c r="L100" s="166"/>
+      <c r="M100" s="159"/>
       <c r="N100" s="153"/>
     </row>
     <row r="101" spans="1:14">
@@ -6449,8 +6452,8 @@
       <c r="K101" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L101" s="147"/>
-      <c r="M101" s="156"/>
+      <c r="L101" s="166"/>
+      <c r="M101" s="159"/>
       <c r="N101" s="153"/>
     </row>
     <row r="102" spans="1:14">
@@ -6484,8 +6487,8 @@
       <c r="K102" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L102" s="147"/>
-      <c r="M102" s="156"/>
+      <c r="L102" s="166"/>
+      <c r="M102" s="159"/>
       <c r="N102" s="153"/>
     </row>
     <row r="103" spans="1:14">
@@ -6520,8 +6523,8 @@
       <c r="K103" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="L103" s="148"/>
-      <c r="M103" s="157"/>
+      <c r="L103" s="167"/>
+      <c r="M103" s="160"/>
       <c r="N103" s="154"/>
     </row>
     <row r="104" spans="1:14">
@@ -6597,10 +6600,10 @@
       <c r="K105" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L105" s="146" t="s">
+      <c r="L105" s="165" t="s">
         <v>23</v>
       </c>
-      <c r="M105" s="155" t="s">
+      <c r="M105" s="158" t="s">
         <v>23</v>
       </c>
       <c r="N105" s="152" t="s">
@@ -6638,8 +6641,8 @@
       <c r="K106" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L106" s="147"/>
-      <c r="M106" s="156"/>
+      <c r="L106" s="166"/>
+      <c r="M106" s="159"/>
       <c r="N106" s="153"/>
     </row>
     <row r="107" spans="1:14">
@@ -6673,8 +6676,8 @@
       <c r="K107" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L107" s="147"/>
-      <c r="M107" s="156"/>
+      <c r="L107" s="166"/>
+      <c r="M107" s="159"/>
       <c r="N107" s="153"/>
     </row>
     <row r="108" spans="1:14">
@@ -6708,8 +6711,8 @@
       <c r="K108" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="L108" s="147"/>
-      <c r="M108" s="156"/>
+      <c r="L108" s="166"/>
+      <c r="M108" s="159"/>
       <c r="N108" s="153"/>
     </row>
     <row r="109" spans="1:14">
@@ -6744,8 +6747,8 @@
       <c r="K109" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="L109" s="148"/>
-      <c r="M109" s="157"/>
+      <c r="L109" s="167"/>
+      <c r="M109" s="160"/>
       <c r="N109" s="154"/>
     </row>
     <row r="110" spans="1:14">
@@ -6824,7 +6827,7 @@
       <c r="L111" s="152" t="s">
         <v>24</v>
       </c>
-      <c r="M111" s="155" t="s">
+      <c r="M111" s="158" t="s">
         <v>23</v>
       </c>
       <c r="N111" s="152" t="s">
@@ -6863,7 +6866,7 @@
         <v>21</v>
       </c>
       <c r="L112" s="153"/>
-      <c r="M112" s="156"/>
+      <c r="M112" s="159"/>
       <c r="N112" s="153"/>
     </row>
     <row r="113" spans="1:14">
@@ -6898,7 +6901,7 @@
         <v>21</v>
       </c>
       <c r="L113" s="153"/>
-      <c r="M113" s="156"/>
+      <c r="M113" s="159"/>
       <c r="N113" s="153"/>
     </row>
     <row r="114" spans="1:14">
@@ -6934,7 +6937,7 @@
         <v>21</v>
       </c>
       <c r="L114" s="154"/>
-      <c r="M114" s="157"/>
+      <c r="M114" s="160"/>
       <c r="N114" s="154"/>
     </row>
     <row r="115" spans="1:14">
@@ -7250,6 +7253,87 @@
     </row>
   </sheetData>
   <mergeCells count="97">
+    <mergeCell ref="L33:L35"/>
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="L6:L8"/>
+    <mergeCell ref="L9:L11"/>
+    <mergeCell ref="L13:L15"/>
+    <mergeCell ref="L16:L18"/>
+    <mergeCell ref="L19:L21"/>
+    <mergeCell ref="L22:L24"/>
+    <mergeCell ref="L25:L27"/>
+    <mergeCell ref="L29:L31"/>
+    <mergeCell ref="M19:M21"/>
+    <mergeCell ref="L75:L77"/>
+    <mergeCell ref="L78:L80"/>
+    <mergeCell ref="L81:L83"/>
+    <mergeCell ref="L84:L86"/>
+    <mergeCell ref="L54:L56"/>
+    <mergeCell ref="L57:L59"/>
+    <mergeCell ref="L60:L62"/>
+    <mergeCell ref="L63:L65"/>
+    <mergeCell ref="L68:L70"/>
+    <mergeCell ref="L71:L73"/>
+    <mergeCell ref="L36:L38"/>
+    <mergeCell ref="L39:L41"/>
+    <mergeCell ref="L42:L44"/>
+    <mergeCell ref="L45:L47"/>
+    <mergeCell ref="L48:L50"/>
+    <mergeCell ref="M3:M5"/>
+    <mergeCell ref="M6:M8"/>
+    <mergeCell ref="M9:M11"/>
+    <mergeCell ref="M13:M15"/>
+    <mergeCell ref="M16:M18"/>
+    <mergeCell ref="M39:M41"/>
+    <mergeCell ref="L94:L96"/>
+    <mergeCell ref="L99:L103"/>
+    <mergeCell ref="L105:L109"/>
+    <mergeCell ref="L111:L114"/>
+    <mergeCell ref="L87:L89"/>
+    <mergeCell ref="L91:L93"/>
+    <mergeCell ref="L51:L53"/>
+    <mergeCell ref="M78:M80"/>
+    <mergeCell ref="M42:M44"/>
+    <mergeCell ref="M45:M47"/>
+    <mergeCell ref="M48:M50"/>
+    <mergeCell ref="M51:M53"/>
+    <mergeCell ref="M54:M56"/>
+    <mergeCell ref="M57:M59"/>
+    <mergeCell ref="M60:M62"/>
+    <mergeCell ref="M22:M24"/>
+    <mergeCell ref="M25:M27"/>
+    <mergeCell ref="M29:M31"/>
+    <mergeCell ref="M33:M35"/>
+    <mergeCell ref="M36:M38"/>
+    <mergeCell ref="M63:M65"/>
+    <mergeCell ref="M68:M70"/>
+    <mergeCell ref="M71:M73"/>
+    <mergeCell ref="M75:M77"/>
+    <mergeCell ref="M105:M109"/>
+    <mergeCell ref="M111:M114"/>
+    <mergeCell ref="N3:N5"/>
+    <mergeCell ref="N6:N8"/>
+    <mergeCell ref="N9:N11"/>
+    <mergeCell ref="N13:N15"/>
+    <mergeCell ref="N16:N18"/>
+    <mergeCell ref="N19:N21"/>
+    <mergeCell ref="N22:N24"/>
+    <mergeCell ref="N25:N27"/>
+    <mergeCell ref="M81:M83"/>
+    <mergeCell ref="M84:M86"/>
+    <mergeCell ref="M87:M89"/>
+    <mergeCell ref="M91:M93"/>
+    <mergeCell ref="M94:M96"/>
+    <mergeCell ref="M99:M103"/>
+    <mergeCell ref="N63:N65"/>
+    <mergeCell ref="N51:N53"/>
+    <mergeCell ref="N54:N56"/>
+    <mergeCell ref="N57:N59"/>
+    <mergeCell ref="N29:N31"/>
+    <mergeCell ref="N33:N35"/>
+    <mergeCell ref="N36:N38"/>
+    <mergeCell ref="N39:N41"/>
+    <mergeCell ref="N42:N44"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="N60:N62"/>
     <mergeCell ref="N111:N114"/>
@@ -7266,87 +7350,6 @@
     <mergeCell ref="N105:N109"/>
     <mergeCell ref="N45:N47"/>
     <mergeCell ref="N48:N50"/>
-    <mergeCell ref="N51:N53"/>
-    <mergeCell ref="N54:N56"/>
-    <mergeCell ref="N57:N59"/>
-    <mergeCell ref="N29:N31"/>
-    <mergeCell ref="N33:N35"/>
-    <mergeCell ref="N36:N38"/>
-    <mergeCell ref="N39:N41"/>
-    <mergeCell ref="N42:N44"/>
-    <mergeCell ref="M111:M114"/>
-    <mergeCell ref="N3:N5"/>
-    <mergeCell ref="N6:N8"/>
-    <mergeCell ref="N9:N11"/>
-    <mergeCell ref="N13:N15"/>
-    <mergeCell ref="N16:N18"/>
-    <mergeCell ref="N19:N21"/>
-    <mergeCell ref="N22:N24"/>
-    <mergeCell ref="N25:N27"/>
-    <mergeCell ref="M81:M83"/>
-    <mergeCell ref="M84:M86"/>
-    <mergeCell ref="M87:M89"/>
-    <mergeCell ref="M91:M93"/>
-    <mergeCell ref="M94:M96"/>
-    <mergeCell ref="M99:M103"/>
-    <mergeCell ref="N63:N65"/>
-    <mergeCell ref="M63:M65"/>
-    <mergeCell ref="M68:M70"/>
-    <mergeCell ref="M71:M73"/>
-    <mergeCell ref="M75:M77"/>
-    <mergeCell ref="M105:M109"/>
-    <mergeCell ref="M22:M24"/>
-    <mergeCell ref="M25:M27"/>
-    <mergeCell ref="M29:M31"/>
-    <mergeCell ref="M33:M35"/>
-    <mergeCell ref="M36:M38"/>
-    <mergeCell ref="M39:M41"/>
-    <mergeCell ref="L94:L96"/>
-    <mergeCell ref="L99:L103"/>
-    <mergeCell ref="L105:L109"/>
-    <mergeCell ref="L111:L114"/>
-    <mergeCell ref="L87:L89"/>
-    <mergeCell ref="L91:L93"/>
-    <mergeCell ref="L51:L53"/>
-    <mergeCell ref="M78:M80"/>
-    <mergeCell ref="M42:M44"/>
-    <mergeCell ref="M45:M47"/>
-    <mergeCell ref="M48:M50"/>
-    <mergeCell ref="M51:M53"/>
-    <mergeCell ref="M54:M56"/>
-    <mergeCell ref="M57:M59"/>
-    <mergeCell ref="M60:M62"/>
-    <mergeCell ref="M3:M5"/>
-    <mergeCell ref="M6:M8"/>
-    <mergeCell ref="M9:M11"/>
-    <mergeCell ref="M13:M15"/>
-    <mergeCell ref="M16:M18"/>
-    <mergeCell ref="M19:M21"/>
-    <mergeCell ref="L75:L77"/>
-    <mergeCell ref="L78:L80"/>
-    <mergeCell ref="L81:L83"/>
-    <mergeCell ref="L84:L86"/>
-    <mergeCell ref="L54:L56"/>
-    <mergeCell ref="L57:L59"/>
-    <mergeCell ref="L60:L62"/>
-    <mergeCell ref="L63:L65"/>
-    <mergeCell ref="L68:L70"/>
-    <mergeCell ref="L71:L73"/>
-    <mergeCell ref="L36:L38"/>
-    <mergeCell ref="L39:L41"/>
-    <mergeCell ref="L42:L44"/>
-    <mergeCell ref="L45:L47"/>
-    <mergeCell ref="L48:L50"/>
-    <mergeCell ref="L33:L35"/>
-    <mergeCell ref="L3:L5"/>
-    <mergeCell ref="L6:L8"/>
-    <mergeCell ref="L9:L11"/>
-    <mergeCell ref="L13:L15"/>
-    <mergeCell ref="L16:L18"/>
-    <mergeCell ref="L19:L21"/>
-    <mergeCell ref="L22:L24"/>
-    <mergeCell ref="L25:L27"/>
-    <mergeCell ref="L29:L31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7356,9 +7359,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6F56B36-DF0D-4F9E-BFBE-DAB32168004F}">
   <dimension ref="A1:BC125"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M63" sqref="M63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="S1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AC5" sqref="AC5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7399,54 +7402,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:55" ht="15.75" thickBot="1">
-      <c r="N1" s="169" t="s">
+      <c r="N1" s="187" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="170"/>
-      <c r="P1" s="170"/>
-      <c r="Q1" s="170"/>
-      <c r="R1" s="170"/>
-      <c r="S1" s="171"/>
-      <c r="T1" s="172" t="s">
+      <c r="O1" s="188"/>
+      <c r="P1" s="188"/>
+      <c r="Q1" s="188"/>
+      <c r="R1" s="188"/>
+      <c r="S1" s="189"/>
+      <c r="T1" s="190" t="s">
         <v>191</v>
       </c>
-      <c r="U1" s="173"/>
-      <c r="V1" s="173"/>
-      <c r="W1" s="173"/>
-      <c r="X1" s="173"/>
-      <c r="Y1" s="173"/>
-      <c r="Z1" s="173"/>
-      <c r="AA1" s="173"/>
-      <c r="AB1" s="173"/>
-      <c r="AC1" s="174"/>
+      <c r="U1" s="191"/>
+      <c r="V1" s="191"/>
+      <c r="W1" s="191"/>
+      <c r="X1" s="191"/>
+      <c r="Y1" s="191"/>
+      <c r="Z1" s="191"/>
+      <c r="AA1" s="191"/>
+      <c r="AB1" s="191"/>
+      <c r="AC1" s="192"/>
       <c r="AD1" s="12"/>
       <c r="AE1" s="12"/>
-      <c r="AF1" s="172" t="s">
+      <c r="AF1" s="190" t="s">
         <v>192</v>
       </c>
-      <c r="AG1" s="173"/>
-      <c r="AH1" s="173"/>
-      <c r="AI1" s="173"/>
-      <c r="AJ1" s="173"/>
-      <c r="AK1" s="173"/>
-      <c r="AL1" s="173"/>
-      <c r="AM1" s="173"/>
-      <c r="AN1" s="173"/>
-      <c r="AO1" s="174"/>
+      <c r="AG1" s="191"/>
+      <c r="AH1" s="191"/>
+      <c r="AI1" s="191"/>
+      <c r="AJ1" s="191"/>
+      <c r="AK1" s="191"/>
+      <c r="AL1" s="191"/>
+      <c r="AM1" s="191"/>
+      <c r="AN1" s="191"/>
+      <c r="AO1" s="192"/>
       <c r="AP1" s="12"/>
       <c r="AQ1" s="12"/>
-      <c r="AR1" s="172" t="s">
+      <c r="AR1" s="190" t="s">
         <v>193</v>
       </c>
-      <c r="AS1" s="173"/>
-      <c r="AT1" s="173"/>
-      <c r="AU1" s="173"/>
-      <c r="AV1" s="173"/>
-      <c r="AW1" s="173"/>
-      <c r="AX1" s="173"/>
-      <c r="AY1" s="173"/>
-      <c r="AZ1" s="173"/>
-      <c r="BA1" s="174"/>
+      <c r="AS1" s="191"/>
+      <c r="AT1" s="191"/>
+      <c r="AU1" s="191"/>
+      <c r="AV1" s="191"/>
+      <c r="AW1" s="191"/>
+      <c r="AX1" s="191"/>
+      <c r="AY1" s="191"/>
+      <c r="AZ1" s="191"/>
+      <c r="BA1" s="192"/>
       <c r="BB1" s="12"/>
       <c r="BC1" s="129"/>
     </row>
@@ -7695,7 +7698,7 @@
       <c r="AC3" s="125" t="s">
         <v>24</v>
       </c>
-      <c r="AD3" s="178" t="s">
+      <c r="AD3" s="194" t="s">
         <v>22</v>
       </c>
       <c r="AE3" s="117" t="s">
@@ -7721,7 +7724,7 @@
       <c r="AO3" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="AP3" s="181" t="s">
+      <c r="AP3" s="195" t="s">
         <v>23</v>
       </c>
       <c r="AQ3" s="105"/>
@@ -7745,7 +7748,7 @@
       <c r="BA3" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="BB3" s="175" t="s">
+      <c r="BB3" s="193" t="s">
         <v>24</v>
       </c>
       <c r="BC3" s="105"/>
@@ -7823,7 +7826,7 @@
       <c r="AC4" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="AD4" s="179"/>
+      <c r="AD4" s="182"/>
       <c r="AE4" s="106"/>
       <c r="AF4" s="43" t="s">
         <v>226</v>
@@ -7855,7 +7858,7 @@
       <c r="AO4" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AP4" s="182"/>
+      <c r="AP4" s="170"/>
       <c r="AQ4" s="106"/>
       <c r="AR4" s="43" t="s">
         <v>227</v>
@@ -7872,7 +7875,7 @@
       <c r="BA4" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB4" s="176"/>
+      <c r="BB4" s="173"/>
       <c r="BC4" s="106"/>
     </row>
     <row r="5" spans="1:55">
@@ -7953,7 +7956,7 @@
       <c r="AC5" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="AD5" s="180"/>
+      <c r="AD5" s="183"/>
       <c r="AE5" s="107"/>
       <c r="AF5" s="44" t="s">
         <v>226</v>
@@ -7979,7 +7982,7 @@
       <c r="AO5" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="AP5" s="183"/>
+      <c r="AP5" s="171"/>
       <c r="AQ5" s="107"/>
       <c r="AR5" s="44" t="s">
         <v>227</v>
@@ -8001,7 +8004,7 @@
       <c r="BA5" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BB5" s="177"/>
+      <c r="BB5" s="174"/>
       <c r="BC5" s="107"/>
     </row>
     <row r="6" spans="1:55">
@@ -8082,7 +8085,7 @@
       <c r="AC6" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="AD6" s="184" t="s">
+      <c r="AD6" s="172" t="s">
         <v>24</v>
       </c>
       <c r="AE6" s="108"/>
@@ -8110,7 +8113,7 @@
       <c r="AO6" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AP6" s="185" t="s">
+      <c r="AP6" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AQ6" s="118" t="s">
@@ -8136,7 +8139,7 @@
       <c r="BA6" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="BB6" s="184" t="s">
+      <c r="BB6" s="172" t="s">
         <v>24</v>
       </c>
       <c r="BC6" s="106"/>
@@ -8219,7 +8222,7 @@
       <c r="AC7" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="AD7" s="176"/>
+      <c r="AD7" s="173"/>
       <c r="AE7" s="106"/>
       <c r="AF7" s="43" t="s">
         <v>223</v>
@@ -8245,7 +8248,7 @@
       <c r="AO7" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AP7" s="182"/>
+      <c r="AP7" s="170"/>
       <c r="AQ7" s="119" t="s">
         <v>229</v>
       </c>
@@ -8264,7 +8267,7 @@
       <c r="BA7" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB7" s="176"/>
+      <c r="BB7" s="173"/>
       <c r="BC7" s="106"/>
     </row>
     <row r="8" spans="1:55">
@@ -8345,7 +8348,7 @@
       <c r="AC8" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="AD8" s="177"/>
+      <c r="AD8" s="174"/>
       <c r="AE8" s="107"/>
       <c r="AF8" s="44" t="s">
         <v>223</v>
@@ -8375,7 +8378,7 @@
       <c r="AO8" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="AP8" s="183"/>
+      <c r="AP8" s="171"/>
       <c r="AQ8" s="120" t="s">
         <v>228</v>
       </c>
@@ -8399,7 +8402,7 @@
       <c r="BA8" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BB8" s="177"/>
+      <c r="BB8" s="174"/>
       <c r="BC8" s="107"/>
     </row>
     <row r="9" spans="1:55">
@@ -8488,7 +8491,7 @@
       <c r="AC9" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AD9" s="185" t="s">
+      <c r="AD9" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AE9" s="108"/>
@@ -8520,7 +8523,7 @@
       <c r="AO9" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AP9" s="185" t="s">
+      <c r="AP9" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AQ9" s="108"/>
@@ -8544,7 +8547,7 @@
       <c r="BA9" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="BB9" s="184" t="s">
+      <c r="BB9" s="172" t="s">
         <v>24</v>
       </c>
       <c r="BC9" s="106"/>
@@ -8637,7 +8640,7 @@
       <c r="AC10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AD10" s="182"/>
+      <c r="AD10" s="170"/>
       <c r="AE10" s="106"/>
       <c r="AF10" s="43" t="s">
         <v>226</v>
@@ -8669,7 +8672,7 @@
       <c r="AO10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AP10" s="182"/>
+      <c r="AP10" s="170"/>
       <c r="AQ10" s="106"/>
       <c r="AR10" s="43" t="s">
         <v>227</v>
@@ -8686,7 +8689,7 @@
       <c r="BA10" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB10" s="176"/>
+      <c r="BB10" s="173"/>
       <c r="BC10" s="106"/>
     </row>
     <row r="11" spans="1:55">
@@ -8775,7 +8778,7 @@
       <c r="AC11" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="AD11" s="183"/>
+      <c r="AD11" s="171"/>
       <c r="AE11" s="107"/>
       <c r="AF11" s="44" t="s">
         <v>223</v>
@@ -8805,7 +8808,7 @@
       <c r="AO11" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="AP11" s="183"/>
+      <c r="AP11" s="171"/>
       <c r="AQ11" s="107"/>
       <c r="AR11" s="44" t="s">
         <v>224</v>
@@ -8827,7 +8830,7 @@
       <c r="BA11" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BB11" s="177"/>
+      <c r="BB11" s="174"/>
       <c r="BC11" s="107"/>
     </row>
     <row r="12" spans="1:55">
@@ -9030,7 +9033,7 @@
       <c r="AC13" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AD13" s="185" t="s">
+      <c r="AD13" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AE13" s="108"/>
@@ -9064,7 +9067,7 @@
       <c r="AO13" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AP13" s="185" t="s">
+      <c r="AP13" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AQ13" s="108"/>
@@ -9088,7 +9091,7 @@
       <c r="BA13" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="BB13" s="184" t="s">
+      <c r="BB13" s="172" t="s">
         <v>24</v>
       </c>
       <c r="BC13" s="106"/>
@@ -9181,7 +9184,7 @@
       <c r="AC14" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AD14" s="182"/>
+      <c r="AD14" s="170"/>
       <c r="AE14" s="106"/>
       <c r="AF14" s="43" t="s">
         <v>223</v>
@@ -9213,7 +9216,7 @@
       <c r="AO14" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AP14" s="182"/>
+      <c r="AP14" s="170"/>
       <c r="AQ14" s="106"/>
       <c r="AR14" s="43" t="s">
         <v>224</v>
@@ -9230,7 +9233,7 @@
       <c r="BA14" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB14" s="176"/>
+      <c r="BB14" s="173"/>
       <c r="BC14" s="106"/>
     </row>
     <row r="15" spans="1:55">
@@ -9321,7 +9324,7 @@
       <c r="AC15" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AD15" s="183"/>
+      <c r="AD15" s="171"/>
       <c r="AE15" s="107"/>
       <c r="AF15" s="44" t="s">
         <v>226</v>
@@ -9351,7 +9354,7 @@
       <c r="AO15" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="AP15" s="183"/>
+      <c r="AP15" s="171"/>
       <c r="AQ15" s="107"/>
       <c r="AR15" s="44" t="s">
         <v>227</v>
@@ -9373,7 +9376,7 @@
       <c r="BA15" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BB15" s="177"/>
+      <c r="BB15" s="174"/>
       <c r="BC15" s="107"/>
     </row>
     <row r="16" spans="1:55">
@@ -9464,7 +9467,7 @@
       <c r="AC16" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AD16" s="185" t="s">
+      <c r="AD16" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AE16" s="108"/>
@@ -9498,7 +9501,7 @@
       <c r="AO16" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AP16" s="185" t="s">
+      <c r="AP16" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AQ16" s="108"/>
@@ -9522,7 +9525,7 @@
       <c r="BA16" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="BB16" s="186" t="s">
+      <c r="BB16" s="184" t="s">
         <v>24</v>
       </c>
       <c r="BC16" s="132"/>
@@ -9615,7 +9618,7 @@
       <c r="AC17" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AD17" s="182"/>
+      <c r="AD17" s="170"/>
       <c r="AE17" s="106"/>
       <c r="AF17" s="43" t="s">
         <v>226</v>
@@ -9647,7 +9650,7 @@
       <c r="AO17" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AP17" s="182"/>
+      <c r="AP17" s="170"/>
       <c r="AQ17" s="106"/>
       <c r="AR17" s="43" t="s">
         <v>227</v>
@@ -9664,7 +9667,7 @@
       <c r="BA17" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB17" s="187"/>
+      <c r="BB17" s="185"/>
       <c r="BC17" s="132"/>
     </row>
     <row r="18" spans="1:55">
@@ -9755,7 +9758,7 @@
       <c r="AC18" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AD18" s="183"/>
+      <c r="AD18" s="171"/>
       <c r="AE18" s="107"/>
       <c r="AF18" s="44" t="s">
         <v>226</v>
@@ -9787,7 +9790,7 @@
       <c r="AO18" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AP18" s="183"/>
+      <c r="AP18" s="171"/>
       <c r="AQ18" s="107"/>
       <c r="AR18" s="44" t="s">
         <v>227</v>
@@ -9809,7 +9812,7 @@
       <c r="BA18" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BB18" s="188"/>
+      <c r="BB18" s="186"/>
       <c r="BC18" s="107"/>
     </row>
     <row r="19" spans="1:55">
@@ -9900,7 +9903,7 @@
       <c r="AC19" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AD19" s="185" t="s">
+      <c r="AD19" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AE19" s="108"/>
@@ -9934,7 +9937,7 @@
       <c r="AO19" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AP19" s="185" t="s">
+      <c r="AP19" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AQ19" s="108"/>
@@ -9958,7 +9961,7 @@
       <c r="BA19" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="BB19" s="186" t="s">
+      <c r="BB19" s="184" t="s">
         <v>24</v>
       </c>
       <c r="BC19" s="132"/>
@@ -10051,7 +10054,7 @@
       <c r="AC20" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AD20" s="182"/>
+      <c r="AD20" s="170"/>
       <c r="AE20" s="106"/>
       <c r="AF20" s="43" t="s">
         <v>226</v>
@@ -10083,7 +10086,7 @@
       <c r="AO20" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AP20" s="182"/>
+      <c r="AP20" s="170"/>
       <c r="AQ20" s="106"/>
       <c r="AR20" s="43" t="s">
         <v>227</v>
@@ -10100,7 +10103,7 @@
       <c r="BA20" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB20" s="187"/>
+      <c r="BB20" s="185"/>
       <c r="BC20" s="132"/>
     </row>
     <row r="21" spans="1:55">
@@ -10191,7 +10194,7 @@
       <c r="AC21" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AD21" s="183"/>
+      <c r="AD21" s="171"/>
       <c r="AE21" s="107"/>
       <c r="AF21" s="44" t="s">
         <v>223</v>
@@ -10223,7 +10226,7 @@
       <c r="AO21" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AP21" s="183"/>
+      <c r="AP21" s="171"/>
       <c r="AQ21" s="107"/>
       <c r="AR21" s="44" t="s">
         <v>224</v>
@@ -10245,7 +10248,7 @@
       <c r="BA21" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BB21" s="188"/>
+      <c r="BB21" s="186"/>
       <c r="BC21" s="107"/>
     </row>
     <row r="22" spans="1:55">
@@ -10334,7 +10337,7 @@
       <c r="AC22" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AD22" s="185" t="s">
+      <c r="AD22" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AE22" s="108"/>
@@ -10366,7 +10369,7 @@
       <c r="AO22" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AP22" s="185" t="s">
+      <c r="AP22" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AQ22" s="108"/>
@@ -10390,7 +10393,7 @@
       <c r="BA22" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="BB22" s="186" t="s">
+      <c r="BB22" s="184" t="s">
         <v>24</v>
       </c>
       <c r="BC22" s="132"/>
@@ -10483,7 +10486,7 @@
       <c r="AC23" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AD23" s="182"/>
+      <c r="AD23" s="170"/>
       <c r="AE23" s="106"/>
       <c r="AF23" s="43" t="s">
         <v>226</v>
@@ -10515,7 +10518,7 @@
       <c r="AO23" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AP23" s="182"/>
+      <c r="AP23" s="170"/>
       <c r="AQ23" s="106"/>
       <c r="AR23" s="43" t="s">
         <v>227</v>
@@ -10532,7 +10535,7 @@
       <c r="BA23" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB23" s="187"/>
+      <c r="BB23" s="185"/>
       <c r="BC23" s="132"/>
     </row>
     <row r="24" spans="1:55">
@@ -10617,7 +10620,7 @@
       <c r="AC24" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="AD24" s="183"/>
+      <c r="AD24" s="171"/>
       <c r="AE24" s="107"/>
       <c r="AF24" s="44" t="s">
         <v>226</v>
@@ -10649,7 +10652,7 @@
       <c r="AO24" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AP24" s="183"/>
+      <c r="AP24" s="171"/>
       <c r="AQ24" s="107"/>
       <c r="AR24" s="44" t="s">
         <v>227</v>
@@ -10671,7 +10674,7 @@
       <c r="BA24" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BB24" s="188"/>
+      <c r="BB24" s="186"/>
       <c r="BC24" s="107"/>
     </row>
     <row r="25" spans="1:55">
@@ -10762,7 +10765,7 @@
       <c r="AC25" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AD25" s="185" t="s">
+      <c r="AD25" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AE25" s="108"/>
@@ -10796,7 +10799,7 @@
       <c r="AO25" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AP25" s="185" t="s">
+      <c r="AP25" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AQ25" s="108"/>
@@ -10820,7 +10823,7 @@
       <c r="BA25" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="BB25" s="184" t="s">
+      <c r="BB25" s="172" t="s">
         <v>24</v>
       </c>
       <c r="BC25" s="108"/>
@@ -10913,7 +10916,7 @@
       <c r="AC26" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AD26" s="182"/>
+      <c r="AD26" s="170"/>
       <c r="AE26" s="106"/>
       <c r="AF26" s="43" t="s">
         <v>226</v>
@@ -10945,7 +10948,7 @@
       <c r="AO26" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AP26" s="182"/>
+      <c r="AP26" s="170"/>
       <c r="AQ26" s="106"/>
       <c r="AR26" s="43" t="s">
         <v>227</v>
@@ -10962,7 +10965,7 @@
       <c r="BA26" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB26" s="176"/>
+      <c r="BB26" s="173"/>
       <c r="BC26" s="106"/>
     </row>
     <row r="27" spans="1:55">
@@ -11053,7 +11056,7 @@
       <c r="AC27" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AD27" s="183"/>
+      <c r="AD27" s="171"/>
       <c r="AE27" s="107"/>
       <c r="AF27" s="44" t="s">
         <v>226</v>
@@ -11085,7 +11088,7 @@
       <c r="AO27" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AP27" s="183"/>
+      <c r="AP27" s="171"/>
       <c r="AQ27" s="107"/>
       <c r="AR27" s="44" t="s">
         <v>227</v>
@@ -11107,7 +11110,7 @@
       <c r="BA27" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BB27" s="177"/>
+      <c r="BB27" s="174"/>
       <c r="BC27" s="107"/>
     </row>
     <row r="28" spans="1:55">
@@ -11306,7 +11309,7 @@
       <c r="AC29" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="AD29" s="184" t="s">
+      <c r="AD29" s="172" t="s">
         <v>24</v>
       </c>
       <c r="AE29" s="108"/>
@@ -11330,7 +11333,7 @@
       <c r="AO29" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="AP29" s="184" t="s">
+      <c r="AP29" s="172" t="s">
         <v>24</v>
       </c>
       <c r="AQ29" s="108"/>
@@ -11354,7 +11357,7 @@
       <c r="BA29" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="BB29" s="189" t="s">
+      <c r="BB29" s="178" t="s">
         <v>22</v>
       </c>
       <c r="BC29" s="119" t="s">
@@ -11434,7 +11437,7 @@
       <c r="AC30" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="AD30" s="176"/>
+      <c r="AD30" s="173"/>
       <c r="AE30" s="106"/>
       <c r="AF30" s="43" t="s">
         <v>226</v>
@@ -11456,7 +11459,7 @@
       <c r="AO30" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="AP30" s="176"/>
+      <c r="AP30" s="173"/>
       <c r="AQ30" s="106"/>
       <c r="AR30" s="43" t="s">
         <v>227</v>
@@ -11473,7 +11476,7 @@
       <c r="BA30" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB30" s="190"/>
+      <c r="BB30" s="179"/>
       <c r="BC30" s="119" t="s">
         <v>230</v>
       </c>
@@ -11556,7 +11559,7 @@
       <c r="AC31" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="AD31" s="177"/>
+      <c r="AD31" s="174"/>
       <c r="AE31" s="107"/>
       <c r="AF31" s="44" t="s">
         <v>226</v>
@@ -11578,7 +11581,7 @@
       <c r="AO31" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="AP31" s="177"/>
+      <c r="AP31" s="174"/>
       <c r="AQ31" s="107"/>
       <c r="AR31" s="44" t="s">
         <v>227</v>
@@ -11608,7 +11611,7 @@
       <c r="BA31" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="BB31" s="191"/>
+      <c r="BB31" s="180"/>
       <c r="BC31" s="127" t="s">
         <v>231</v>
       </c>
@@ -11836,7 +11839,7 @@
       <c r="AC33" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AD33" s="185" t="s">
+      <c r="AD33" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AE33" s="108"/>
@@ -11870,7 +11873,7 @@
       <c r="AO33" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AP33" s="185" t="s">
+      <c r="AP33" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AQ33" s="108"/>
@@ -11894,7 +11897,7 @@
       <c r="BA33" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="BB33" s="184" t="s">
+      <c r="BB33" s="172" t="s">
         <v>24</v>
       </c>
       <c r="BC33" s="106"/>
@@ -11987,7 +11990,7 @@
       <c r="AC34" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AD34" s="182"/>
+      <c r="AD34" s="170"/>
       <c r="AE34" s="106"/>
       <c r="AF34" s="43" t="s">
         <v>226</v>
@@ -12017,7 +12020,7 @@
       <c r="AO34" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AP34" s="182"/>
+      <c r="AP34" s="170"/>
       <c r="AQ34" s="106"/>
       <c r="AR34" s="43" t="s">
         <v>227</v>
@@ -12034,7 +12037,7 @@
       <c r="BA34" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB34" s="176"/>
+      <c r="BB34" s="173"/>
       <c r="BC34" s="106"/>
     </row>
     <row r="35" spans="1:55">
@@ -12125,7 +12128,7 @@
       <c r="AC35" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AD35" s="183"/>
+      <c r="AD35" s="171"/>
       <c r="AE35" s="107"/>
       <c r="AF35" s="44" t="s">
         <v>226</v>
@@ -12151,7 +12154,7 @@
       <c r="AO35" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="AP35" s="183"/>
+      <c r="AP35" s="171"/>
       <c r="AQ35" s="107"/>
       <c r="AR35" s="44" t="s">
         <v>227</v>
@@ -12173,7 +12176,7 @@
       <c r="BA35" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BB35" s="177"/>
+      <c r="BB35" s="174"/>
       <c r="BC35" s="107"/>
     </row>
     <row r="36" spans="1:55">
@@ -12264,7 +12267,7 @@
       <c r="AC36" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AD36" s="185" t="s">
+      <c r="AD36" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AE36" s="108"/>
@@ -12298,7 +12301,7 @@
       <c r="AO36" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AP36" s="185" t="s">
+      <c r="AP36" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AQ36" s="108"/>
@@ -12322,7 +12325,7 @@
       <c r="BA36" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="BB36" s="189" t="s">
+      <c r="BB36" s="178" t="s">
         <v>22</v>
       </c>
       <c r="BC36" s="119" t="s">
@@ -12417,7 +12420,7 @@
       <c r="AC37" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AD37" s="182"/>
+      <c r="AD37" s="170"/>
       <c r="AE37" s="106"/>
       <c r="AF37" s="43" t="s">
         <v>226</v>
@@ -12449,7 +12452,7 @@
       <c r="AO37" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AP37" s="182"/>
+      <c r="AP37" s="170"/>
       <c r="AQ37" s="106"/>
       <c r="AR37" s="43" t="s">
         <v>227</v>
@@ -12472,7 +12475,7 @@
       <c r="BA37" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="BB37" s="190"/>
+      <c r="BB37" s="179"/>
       <c r="BC37" s="136" t="s">
         <v>231</v>
       </c>
@@ -12565,7 +12568,7 @@
       <c r="AC38" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AD38" s="183"/>
+      <c r="AD38" s="171"/>
       <c r="AE38" s="107"/>
       <c r="AF38" s="44" t="s">
         <v>226</v>
@@ -12597,7 +12600,7 @@
       <c r="AO38" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AP38" s="183"/>
+      <c r="AP38" s="171"/>
       <c r="AQ38" s="107"/>
       <c r="AR38" s="44" t="s">
         <v>227</v>
@@ -12619,7 +12622,7 @@
       <c r="BA38" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BB38" s="191"/>
+      <c r="BB38" s="180"/>
       <c r="BC38" s="120" t="s">
         <v>230</v>
       </c>
@@ -12712,7 +12715,7 @@
       <c r="AC39" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AD39" s="185" t="s">
+      <c r="AD39" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AE39" s="108"/>
@@ -12746,7 +12749,7 @@
       <c r="AO39" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AP39" s="185" t="s">
+      <c r="AP39" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AQ39" s="108"/>
@@ -12774,7 +12777,7 @@
       <c r="BA39" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="BB39" s="192" t="s">
+      <c r="BB39" s="181" t="s">
         <v>22</v>
       </c>
       <c r="BC39" s="134" t="s">
@@ -12869,7 +12872,7 @@
       <c r="AC40" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AD40" s="182"/>
+      <c r="AD40" s="170"/>
       <c r="AE40" s="106"/>
       <c r="AF40" s="43" t="s">
         <v>226</v>
@@ -12901,7 +12904,7 @@
       <c r="AO40" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AP40" s="182"/>
+      <c r="AP40" s="170"/>
       <c r="AQ40" s="106"/>
       <c r="AR40" s="43" t="s">
         <v>227</v>
@@ -12918,7 +12921,7 @@
       <c r="BA40" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB40" s="179"/>
+      <c r="BB40" s="182"/>
       <c r="BC40" s="119" t="s">
         <v>230</v>
       </c>
@@ -13011,7 +13014,7 @@
       <c r="AC41" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AD41" s="183"/>
+      <c r="AD41" s="171"/>
       <c r="AE41" s="107"/>
       <c r="AF41" s="44" t="s">
         <v>226</v>
@@ -13043,7 +13046,7 @@
       <c r="AO41" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AP41" s="183"/>
+      <c r="AP41" s="171"/>
       <c r="AQ41" s="107"/>
       <c r="AR41" s="44" t="s">
         <v>227</v>
@@ -13069,7 +13072,7 @@
       <c r="BA41" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="BB41" s="180"/>
+      <c r="BB41" s="183"/>
       <c r="BC41" s="135" t="s">
         <v>231</v>
       </c>
@@ -13162,7 +13165,7 @@
       <c r="AC42" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AD42" s="185" t="s">
+      <c r="AD42" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AE42" s="108"/>
@@ -13196,7 +13199,7 @@
       <c r="AO42" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AP42" s="185" t="s">
+      <c r="AP42" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AQ42" s="108"/>
@@ -13220,7 +13223,7 @@
       <c r="BA42" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="BB42" s="184" t="s">
+      <c r="BB42" s="172" t="s">
         <v>24</v>
       </c>
       <c r="BC42" s="106"/>
@@ -13313,7 +13316,7 @@
       <c r="AC43" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AD43" s="182"/>
+      <c r="AD43" s="170"/>
       <c r="AE43" s="106"/>
       <c r="AF43" s="43" t="s">
         <v>226</v>
@@ -13345,7 +13348,7 @@
       <c r="AO43" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AP43" s="182"/>
+      <c r="AP43" s="170"/>
       <c r="AQ43" s="106"/>
       <c r="AR43" s="43" t="s">
         <v>227</v>
@@ -13362,7 +13365,7 @@
       <c r="BA43" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB43" s="176"/>
+      <c r="BB43" s="173"/>
       <c r="BC43" s="106"/>
     </row>
     <row r="44" spans="1:55">
@@ -13453,7 +13456,7 @@
       <c r="AC44" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AD44" s="183"/>
+      <c r="AD44" s="171"/>
       <c r="AE44" s="107"/>
       <c r="AF44" s="44" t="s">
         <v>223</v>
@@ -13483,7 +13486,7 @@
       <c r="AO44" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="AP44" s="183"/>
+      <c r="AP44" s="171"/>
       <c r="AQ44" s="107"/>
       <c r="AR44" s="44" t="s">
         <v>224</v>
@@ -13505,7 +13508,7 @@
       <c r="BA44" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BB44" s="177"/>
+      <c r="BB44" s="174"/>
       <c r="BC44" s="107"/>
     </row>
     <row r="45" spans="1:55">
@@ -13594,7 +13597,7 @@
       <c r="AC45" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AD45" s="185" t="s">
+      <c r="AD45" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AE45" s="108"/>
@@ -13626,7 +13629,7 @@
       <c r="AO45" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AP45" s="185" t="s">
+      <c r="AP45" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AQ45" s="108"/>
@@ -13650,7 +13653,7 @@
       <c r="BA45" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="BB45" s="184" t="s">
+      <c r="BB45" s="172" t="s">
         <v>24</v>
       </c>
       <c r="BC45" s="106"/>
@@ -13743,7 +13746,7 @@
       <c r="AC46" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AD46" s="182"/>
+      <c r="AD46" s="170"/>
       <c r="AE46" s="106"/>
       <c r="AF46" s="43" t="s">
         <v>226</v>
@@ -13775,7 +13778,7 @@
       <c r="AO46" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AP46" s="182"/>
+      <c r="AP46" s="170"/>
       <c r="AQ46" s="106"/>
       <c r="AR46" s="43" t="s">
         <v>227</v>
@@ -13792,7 +13795,7 @@
       <c r="BA46" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB46" s="176"/>
+      <c r="BB46" s="173"/>
       <c r="BC46" s="106"/>
     </row>
     <row r="47" spans="1:55">
@@ -13883,7 +13886,7 @@
       <c r="AC47" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AD47" s="183"/>
+      <c r="AD47" s="171"/>
       <c r="AE47" s="107"/>
       <c r="AF47" s="44" t="s">
         <v>226</v>
@@ -13915,7 +13918,7 @@
       <c r="AO47" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AP47" s="183"/>
+      <c r="AP47" s="171"/>
       <c r="AQ47" s="107"/>
       <c r="AR47" s="44" t="s">
         <v>227</v>
@@ -13937,7 +13940,7 @@
       <c r="BA47" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BB47" s="177"/>
+      <c r="BB47" s="174"/>
       <c r="BC47" s="107"/>
     </row>
     <row r="48" spans="1:55">
@@ -14024,7 +14027,7 @@
       <c r="AC48" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AD48" s="185" t="s">
+      <c r="AD48" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AE48" s="108"/>
@@ -14058,7 +14061,7 @@
       <c r="AO48" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AP48" s="185" t="s">
+      <c r="AP48" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AQ48" s="108"/>
@@ -14082,7 +14085,7 @@
       <c r="BA48" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="BB48" s="184" t="s">
+      <c r="BB48" s="172" t="s">
         <v>24</v>
       </c>
       <c r="BC48" s="106"/>
@@ -14167,7 +14170,7 @@
       <c r="AC49" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AD49" s="182"/>
+      <c r="AD49" s="170"/>
       <c r="AE49" s="106"/>
       <c r="AF49" s="43" t="s">
         <v>223</v>
@@ -14199,7 +14202,7 @@
       <c r="AO49" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AP49" s="182"/>
+      <c r="AP49" s="170"/>
       <c r="AQ49" s="106"/>
       <c r="AR49" s="43" t="s">
         <v>224</v>
@@ -14216,7 +14219,7 @@
       <c r="BA49" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB49" s="176"/>
+      <c r="BB49" s="173"/>
       <c r="BC49" s="106"/>
     </row>
     <row r="50" spans="1:55">
@@ -14303,7 +14306,7 @@
       <c r="AC50" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AD50" s="183"/>
+      <c r="AD50" s="171"/>
       <c r="AE50" s="107"/>
       <c r="AF50" s="44" t="s">
         <v>223</v>
@@ -14335,7 +14338,7 @@
       <c r="AO50" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AP50" s="183"/>
+      <c r="AP50" s="171"/>
       <c r="AQ50" s="107"/>
       <c r="AR50" s="44" t="s">
         <v>224</v>
@@ -14357,7 +14360,7 @@
       <c r="BA50" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BB50" s="177"/>
+      <c r="BB50" s="174"/>
       <c r="BC50" s="107"/>
     </row>
     <row r="51" spans="1:55">
@@ -14438,7 +14441,7 @@
       <c r="AC51" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="AD51" s="184" t="s">
+      <c r="AD51" s="172" t="s">
         <v>24</v>
       </c>
       <c r="AE51" s="108"/>
@@ -14462,7 +14465,7 @@
       <c r="AO51" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="AP51" s="184" t="s">
+      <c r="AP51" s="172" t="s">
         <v>24</v>
       </c>
       <c r="AQ51" s="108"/>
@@ -14486,7 +14489,7 @@
       <c r="BA51" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="BB51" s="184" t="s">
+      <c r="BB51" s="172" t="s">
         <v>24</v>
       </c>
       <c r="BC51" s="106"/>
@@ -14569,7 +14572,7 @@
       <c r="AC52" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="AD52" s="176"/>
+      <c r="AD52" s="173"/>
       <c r="AE52" s="106"/>
       <c r="AF52" s="43" t="s">
         <v>223</v>
@@ -14591,7 +14594,7 @@
       <c r="AO52" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="AP52" s="176"/>
+      <c r="AP52" s="173"/>
       <c r="AQ52" s="106"/>
       <c r="AR52" s="43" t="s">
         <v>224</v>
@@ -14608,7 +14611,7 @@
       <c r="BA52" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB52" s="176"/>
+      <c r="BB52" s="173"/>
       <c r="BC52" s="106"/>
     </row>
     <row r="53" spans="1:55">
@@ -14689,7 +14692,7 @@
       <c r="AC53" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="AD53" s="177"/>
+      <c r="AD53" s="174"/>
       <c r="AE53" s="107"/>
       <c r="AF53" s="44" t="s">
         <v>223</v>
@@ -14711,7 +14714,7 @@
       <c r="AO53" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="AP53" s="177"/>
+      <c r="AP53" s="174"/>
       <c r="AQ53" s="107"/>
       <c r="AR53" s="44" t="s">
         <v>224</v>
@@ -14733,7 +14736,7 @@
       <c r="BA53" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BB53" s="177"/>
+      <c r="BB53" s="174"/>
       <c r="BC53" s="107"/>
     </row>
     <row r="54" spans="1:55">
@@ -14814,7 +14817,7 @@
       <c r="AC54" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="AD54" s="184" t="s">
+      <c r="AD54" s="172" t="s">
         <v>24</v>
       </c>
       <c r="AE54" s="108"/>
@@ -14838,7 +14841,7 @@
       <c r="AO54" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="AP54" s="185" t="s">
+      <c r="AP54" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AQ54" s="108"/>
@@ -14862,7 +14865,7 @@
       <c r="BA54" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="BB54" s="184" t="s">
+      <c r="BB54" s="172" t="s">
         <v>24</v>
       </c>
       <c r="BC54" s="106"/>
@@ -14940,7 +14943,7 @@
       <c r="AC55" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="AD55" s="176"/>
+      <c r="AD55" s="173"/>
       <c r="AE55" s="106"/>
       <c r="AF55" s="43" t="s">
         <v>226</v>
@@ -14962,7 +14965,7 @@
       <c r="AO55" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="AP55" s="182"/>
+      <c r="AP55" s="170"/>
       <c r="AQ55" s="106"/>
       <c r="AR55" s="43" t="s">
         <v>227</v>
@@ -14979,7 +14982,7 @@
       <c r="BA55" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB55" s="176"/>
+      <c r="BB55" s="173"/>
       <c r="BC55" s="106"/>
     </row>
     <row r="56" spans="1:55">
@@ -15060,7 +15063,7 @@
       <c r="AC56" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="AD56" s="177"/>
+      <c r="AD56" s="174"/>
       <c r="AE56" s="107"/>
       <c r="AF56" s="44" t="s">
         <v>223</v>
@@ -15092,7 +15095,7 @@
       <c r="AO56" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AP56" s="183"/>
+      <c r="AP56" s="171"/>
       <c r="AQ56" s="107"/>
       <c r="AR56" s="44" t="s">
         <v>224</v>
@@ -15114,7 +15117,7 @@
       <c r="BA56" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BB56" s="177"/>
+      <c r="BB56" s="174"/>
       <c r="BC56" s="107"/>
     </row>
     <row r="57" spans="1:55">
@@ -15203,7 +15206,7 @@
       <c r="AC57" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AD57" s="185" t="s">
+      <c r="AD57" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AE57" s="108"/>
@@ -15235,7 +15238,7 @@
       <c r="AO57" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AP57" s="185" t="s">
+      <c r="AP57" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AQ57" s="108"/>
@@ -15259,7 +15262,7 @@
       <c r="BA57" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="BB57" s="184" t="s">
+      <c r="BB57" s="172" t="s">
         <v>24</v>
       </c>
       <c r="BC57" s="106"/>
@@ -15352,7 +15355,7 @@
       <c r="AC58" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AD58" s="182"/>
+      <c r="AD58" s="170"/>
       <c r="AE58" s="106"/>
       <c r="AF58" s="43" t="s">
         <v>226</v>
@@ -15384,7 +15387,7 @@
       <c r="AO58" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AP58" s="182"/>
+      <c r="AP58" s="170"/>
       <c r="AQ58" s="106"/>
       <c r="AR58" s="43" t="s">
         <v>227</v>
@@ -15401,7 +15404,7 @@
       <c r="BA58" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB58" s="176"/>
+      <c r="BB58" s="173"/>
       <c r="BC58" s="106"/>
     </row>
     <row r="59" spans="1:55">
@@ -15492,7 +15495,7 @@
       <c r="AC59" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AD59" s="183"/>
+      <c r="AD59" s="171"/>
       <c r="AE59" s="107"/>
       <c r="AF59" s="44" t="s">
         <v>223</v>
@@ -15518,7 +15521,7 @@
       <c r="AO59" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="AP59" s="183"/>
+      <c r="AP59" s="171"/>
       <c r="AQ59" s="107"/>
       <c r="AR59" s="44" t="s">
         <v>224</v>
@@ -15540,7 +15543,7 @@
       <c r="BA59" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BB59" s="177"/>
+      <c r="BB59" s="174"/>
       <c r="BC59" s="107"/>
     </row>
     <row r="60" spans="1:55">
@@ -15631,7 +15634,7 @@
       <c r="AC60" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AD60" s="185" t="s">
+      <c r="AD60" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AE60" s="108"/>
@@ -15665,7 +15668,7 @@
       <c r="AO60" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AP60" s="185" t="s">
+      <c r="AP60" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AQ60" s="108"/>
@@ -15689,7 +15692,7 @@
       <c r="BA60" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="BB60" s="189" t="s">
+      <c r="BB60" s="178" t="s">
         <v>22</v>
       </c>
       <c r="BC60" s="119" t="s">
@@ -15784,7 +15787,7 @@
       <c r="AC61" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AD61" s="182"/>
+      <c r="AD61" s="170"/>
       <c r="AE61" s="106"/>
       <c r="AF61" s="43" t="s">
         <v>223</v>
@@ -15814,7 +15817,7 @@
       <c r="AO61" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AP61" s="182"/>
+      <c r="AP61" s="170"/>
       <c r="AQ61" s="106"/>
       <c r="AR61" s="43" t="s">
         <v>224</v>
@@ -15837,7 +15840,7 @@
       <c r="BA61" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="BB61" s="190"/>
+      <c r="BB61" s="179"/>
       <c r="BC61" s="136" t="s">
         <v>231</v>
       </c>
@@ -15930,7 +15933,7 @@
       <c r="AC62" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AD62" s="183"/>
+      <c r="AD62" s="171"/>
       <c r="AE62" s="107"/>
       <c r="AF62" s="44" t="s">
         <v>223</v>
@@ -15956,7 +15959,7 @@
       <c r="AO62" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="AP62" s="183"/>
+      <c r="AP62" s="171"/>
       <c r="AQ62" s="107"/>
       <c r="AR62" s="44" t="s">
         <v>224</v>
@@ -15978,7 +15981,7 @@
       <c r="BA62" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BB62" s="191"/>
+      <c r="BB62" s="180"/>
       <c r="BC62" s="120" t="s">
         <v>230</v>
       </c>
@@ -16071,7 +16074,7 @@
       <c r="AC63" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AD63" s="185" t="s">
+      <c r="AD63" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AE63" s="108"/>
@@ -16105,7 +16108,7 @@
       <c r="AO63" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AP63" s="185" t="s">
+      <c r="AP63" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AQ63" s="108"/>
@@ -16129,7 +16132,7 @@
       <c r="BA63" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="BB63" s="184" t="s">
+      <c r="BB63" s="172" t="s">
         <v>24</v>
       </c>
       <c r="BC63" s="108"/>
@@ -16222,7 +16225,7 @@
       <c r="AC64" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AD64" s="182"/>
+      <c r="AD64" s="170"/>
       <c r="AE64" s="106"/>
       <c r="AF64" s="43" t="s">
         <v>226</v>
@@ -16254,7 +16257,7 @@
       <c r="AO64" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AP64" s="182"/>
+      <c r="AP64" s="170"/>
       <c r="AQ64" s="106"/>
       <c r="AR64" s="43" t="s">
         <v>227</v>
@@ -16271,7 +16274,7 @@
       <c r="BA64" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB64" s="176"/>
+      <c r="BB64" s="173"/>
       <c r="BC64" s="106"/>
     </row>
     <row r="65" spans="1:55">
@@ -16352,7 +16355,7 @@
       <c r="AC65" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="AD65" s="183"/>
+      <c r="AD65" s="171"/>
       <c r="AE65" s="107"/>
       <c r="AF65" s="44" t="s">
         <v>223</v>
@@ -16384,7 +16387,7 @@
       <c r="AO65" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AP65" s="183"/>
+      <c r="AP65" s="171"/>
       <c r="AQ65" s="107"/>
       <c r="AR65" s="44" t="s">
         <v>224</v>
@@ -16406,7 +16409,7 @@
       <c r="BA65" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BB65" s="177"/>
+      <c r="BB65" s="174"/>
       <c r="BC65" s="107"/>
     </row>
     <row r="66" spans="1:55">
@@ -16740,7 +16743,7 @@
       <c r="AC68" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AD68" s="185" t="s">
+      <c r="AD68" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AE68" s="108"/>
@@ -16774,7 +16777,7 @@
       <c r="AO68" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AP68" s="185" t="s">
+      <c r="AP68" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AQ68" s="108"/>
@@ -16798,7 +16801,7 @@
       <c r="BA68" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="BB68" s="184" t="s">
+      <c r="BB68" s="172" t="s">
         <v>24</v>
       </c>
       <c r="BC68" s="108"/>
@@ -16889,7 +16892,7 @@
       <c r="AC69" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AD69" s="182"/>
+      <c r="AD69" s="170"/>
       <c r="AE69" s="106"/>
       <c r="AF69" s="43" t="s">
         <v>223</v>
@@ -16921,7 +16924,7 @@
       <c r="AO69" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AP69" s="182"/>
+      <c r="AP69" s="170"/>
       <c r="AQ69" s="106"/>
       <c r="AR69" s="43" t="s">
         <v>224</v>
@@ -16938,7 +16941,7 @@
       <c r="BA69" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB69" s="176"/>
+      <c r="BB69" s="173"/>
       <c r="BC69" s="106"/>
     </row>
     <row r="70" spans="1:55">
@@ -17029,7 +17032,7 @@
       <c r="AC70" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AD70" s="183"/>
+      <c r="AD70" s="171"/>
       <c r="AE70" s="107"/>
       <c r="AF70" s="44" t="s">
         <v>226</v>
@@ -17059,7 +17062,7 @@
       <c r="AO70" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="AP70" s="183"/>
+      <c r="AP70" s="171"/>
       <c r="AQ70" s="107"/>
       <c r="AR70" s="44" t="s">
         <v>227</v>
@@ -17081,7 +17084,7 @@
       <c r="BA70" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BB70" s="177"/>
+      <c r="BB70" s="174"/>
       <c r="BC70" s="107"/>
     </row>
     <row r="71" spans="1:55">
@@ -17166,7 +17169,7 @@
       <c r="AC71" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AD71" s="185" t="s">
+      <c r="AD71" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AE71" s="118" t="s">
@@ -17200,7 +17203,7 @@
       <c r="AO71" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AP71" s="185" t="s">
+      <c r="AP71" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AQ71" s="118" t="s">
@@ -17230,7 +17233,7 @@
       <c r="BA71" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="BB71" s="192" t="s">
+      <c r="BB71" s="181" t="s">
         <v>22</v>
       </c>
       <c r="BC71" s="136" t="s">
@@ -17319,7 +17322,7 @@
       <c r="AC72" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AD72" s="182"/>
+      <c r="AD72" s="170"/>
       <c r="AE72" s="119" t="s">
         <v>229</v>
       </c>
@@ -17351,7 +17354,7 @@
       <c r="AO72" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AP72" s="182"/>
+      <c r="AP72" s="170"/>
       <c r="AQ72" s="119" t="s">
         <v>229</v>
       </c>
@@ -17376,7 +17379,7 @@
       <c r="BA72" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="BB72" s="179"/>
+      <c r="BB72" s="182"/>
       <c r="BC72" s="136" t="s">
         <v>231</v>
       </c>
@@ -17459,7 +17462,7 @@
       <c r="AC73" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="AD73" s="183"/>
+      <c r="AD73" s="171"/>
       <c r="AE73" s="120" t="s">
         <v>228</v>
       </c>
@@ -17487,7 +17490,7 @@
       <c r="AO73" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="AP73" s="183"/>
+      <c r="AP73" s="171"/>
       <c r="AQ73" s="120" t="s">
         <v>229</v>
       </c>
@@ -17511,7 +17514,7 @@
       <c r="BA73" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BB73" s="180"/>
+      <c r="BB73" s="183"/>
       <c r="BC73" s="119" t="s">
         <v>230</v>
       </c>
@@ -17711,7 +17714,7 @@
       <c r="AC75" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="AD75" s="185" t="s">
+      <c r="AD75" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AE75" s="108"/>
@@ -17743,7 +17746,7 @@
       <c r="AO75" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AP75" s="185" t="s">
+      <c r="AP75" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AQ75" s="108"/>
@@ -17767,7 +17770,7 @@
       <c r="BA75" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="BB75" s="184" t="s">
+      <c r="BB75" s="172" t="s">
         <v>24</v>
       </c>
       <c r="BC75" s="108"/>
@@ -17850,7 +17853,7 @@
       <c r="AC76" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="AD76" s="182"/>
+      <c r="AD76" s="170"/>
       <c r="AE76" s="106"/>
       <c r="AF76" s="43" t="s">
         <v>226</v>
@@ -17882,7 +17885,7 @@
       <c r="AO76" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AP76" s="182"/>
+      <c r="AP76" s="170"/>
       <c r="AQ76" s="106"/>
       <c r="AR76" s="43" t="s">
         <v>227</v>
@@ -17899,7 +17902,7 @@
       <c r="BA76" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB76" s="176"/>
+      <c r="BB76" s="173"/>
       <c r="BC76" s="106"/>
     </row>
     <row r="77" spans="1:55">
@@ -17990,7 +17993,7 @@
       <c r="AC77" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AD77" s="183"/>
+      <c r="AD77" s="171"/>
       <c r="AE77" s="107"/>
       <c r="AF77" s="44" t="s">
         <v>226</v>
@@ -18022,7 +18025,7 @@
       <c r="AO77" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AP77" s="183"/>
+      <c r="AP77" s="171"/>
       <c r="AQ77" s="107"/>
       <c r="AR77" s="44" t="s">
         <v>227</v>
@@ -18044,7 +18047,7 @@
       <c r="BA77" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BB77" s="177"/>
+      <c r="BB77" s="174"/>
       <c r="BC77" s="106"/>
     </row>
     <row r="78" spans="1:55">
@@ -18129,7 +18132,7 @@
       <c r="AC78" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AD78" s="185" t="s">
+      <c r="AD78" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AE78" s="108"/>
@@ -18163,7 +18166,7 @@
       <c r="AO78" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AP78" s="185" t="s">
+      <c r="AP78" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AQ78" s="108"/>
@@ -18187,7 +18190,7 @@
       <c r="BA78" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="BB78" s="184" t="s">
+      <c r="BB78" s="172" t="s">
         <v>24</v>
       </c>
       <c r="BC78" s="108"/>
@@ -18278,7 +18281,7 @@
       <c r="AC79" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AD79" s="182"/>
+      <c r="AD79" s="170"/>
       <c r="AE79" s="106"/>
       <c r="AF79" s="43" t="s">
         <v>226</v>
@@ -18310,7 +18313,7 @@
       <c r="AO79" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AP79" s="182"/>
+      <c r="AP79" s="170"/>
       <c r="AQ79" s="106"/>
       <c r="AR79" s="43" t="s">
         <v>227</v>
@@ -18327,7 +18330,7 @@
       <c r="BA79" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB79" s="176"/>
+      <c r="BB79" s="173"/>
       <c r="BC79" s="106"/>
     </row>
     <row r="80" spans="1:55">
@@ -18418,7 +18421,7 @@
       <c r="AC80" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AD80" s="183"/>
+      <c r="AD80" s="171"/>
       <c r="AE80" s="107"/>
       <c r="AF80" s="44" t="s">
         <v>223</v>
@@ -18450,7 +18453,7 @@
       <c r="AO80" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AP80" s="183"/>
+      <c r="AP80" s="171"/>
       <c r="AQ80" s="107"/>
       <c r="AR80" s="44" t="s">
         <v>224</v>
@@ -18472,7 +18475,7 @@
       <c r="BA80" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BB80" s="177"/>
+      <c r="BB80" s="174"/>
       <c r="BC80" s="106"/>
     </row>
     <row r="81" spans="1:55">
@@ -18563,7 +18566,7 @@
       <c r="AC81" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AD81" s="185" t="s">
+      <c r="AD81" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AE81" s="108"/>
@@ -18597,7 +18600,7 @@
       <c r="AO81" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AP81" s="185" t="s">
+      <c r="AP81" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AQ81" s="108"/>
@@ -18621,7 +18624,7 @@
       <c r="BA81" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="BB81" s="184" t="s">
+      <c r="BB81" s="172" t="s">
         <v>24</v>
       </c>
       <c r="BC81" s="108"/>
@@ -18712,7 +18715,7 @@
       <c r="AC82" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AD82" s="182"/>
+      <c r="AD82" s="170"/>
       <c r="AE82" s="106"/>
       <c r="AF82" s="43" t="s">
         <v>226</v>
@@ -18744,7 +18747,7 @@
       <c r="AO82" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AP82" s="182"/>
+      <c r="AP82" s="170"/>
       <c r="AQ82" s="106"/>
       <c r="AR82" s="43" t="s">
         <v>227</v>
@@ -18761,7 +18764,7 @@
       <c r="BA82" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB82" s="176"/>
+      <c r="BB82" s="173"/>
       <c r="BC82" s="106"/>
     </row>
     <row r="83" spans="1:55">
@@ -18852,7 +18855,7 @@
       <c r="AC83" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AD83" s="183"/>
+      <c r="AD83" s="171"/>
       <c r="AE83" s="107"/>
       <c r="AF83" s="44" t="s">
         <v>223</v>
@@ -18884,7 +18887,7 @@
       <c r="AO83" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AP83" s="183"/>
+      <c r="AP83" s="171"/>
       <c r="AQ83" s="107"/>
       <c r="AR83" s="44" t="s">
         <v>224</v>
@@ -18906,7 +18909,7 @@
       <c r="BA83" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BB83" s="177"/>
+      <c r="BB83" s="174"/>
       <c r="BC83" s="106"/>
     </row>
     <row r="84" spans="1:55">
@@ -18991,7 +18994,7 @@
       <c r="AC84" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AD84" s="185" t="s">
+      <c r="AD84" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AE84" s="118" t="s">
@@ -19021,7 +19024,7 @@
       <c r="AO84" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AP84" s="185" t="s">
+      <c r="AP84" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AQ84" s="108"/>
@@ -19045,7 +19048,7 @@
       <c r="BA84" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="BB84" s="184" t="s">
+      <c r="BB84" s="172" t="s">
         <v>24</v>
       </c>
       <c r="BC84" s="108"/>
@@ -19136,7 +19139,7 @@
       <c r="AC85" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AD85" s="182"/>
+      <c r="AD85" s="170"/>
       <c r="AE85" s="128" t="s">
         <v>235</v>
       </c>
@@ -19170,7 +19173,7 @@
       <c r="AO85" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AP85" s="182"/>
+      <c r="AP85" s="170"/>
       <c r="AQ85" s="106"/>
       <c r="AR85" s="43" t="s">
         <v>224</v>
@@ -19187,7 +19190,7 @@
       <c r="BA85" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB85" s="176"/>
+      <c r="BB85" s="173"/>
       <c r="BC85" s="106"/>
     </row>
     <row r="86" spans="1:55">
@@ -19272,7 +19275,7 @@
       <c r="AC86" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="AD86" s="183"/>
+      <c r="AD86" s="171"/>
       <c r="AE86" s="120" t="s">
         <v>228</v>
       </c>
@@ -19304,7 +19307,7 @@
       <c r="AO86" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="AP86" s="183"/>
+      <c r="AP86" s="171"/>
       <c r="AQ86" s="107"/>
       <c r="AR86" s="44" t="s">
         <v>224</v>
@@ -19326,7 +19329,7 @@
       <c r="BA86" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BB86" s="177"/>
+      <c r="BB86" s="174"/>
       <c r="BC86" s="106"/>
     </row>
     <row r="87" spans="1:55">
@@ -19417,7 +19420,7 @@
       <c r="AC87" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AD87" s="185" t="s">
+      <c r="AD87" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AE87" s="108"/>
@@ -19445,7 +19448,7 @@
       <c r="AO87" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AP87" s="185" t="s">
+      <c r="AP87" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AQ87" s="112" t="s">
@@ -19471,7 +19474,7 @@
       <c r="BA87" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="BB87" s="184" t="s">
+      <c r="BB87" s="172" t="s">
         <v>24</v>
       </c>
       <c r="BC87" s="108"/>
@@ -19554,7 +19557,7 @@
       <c r="AC88" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="AD88" s="182"/>
+      <c r="AD88" s="170"/>
       <c r="AE88" s="106"/>
       <c r="AF88" s="43" t="s">
         <v>223</v>
@@ -19580,7 +19583,7 @@
       <c r="AO88" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AP88" s="182"/>
+      <c r="AP88" s="170"/>
       <c r="AQ88" s="119" t="s">
         <v>228</v>
       </c>
@@ -19599,7 +19602,7 @@
       <c r="BA88" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB88" s="176"/>
+      <c r="BB88" s="173"/>
       <c r="BC88" s="106"/>
     </row>
     <row r="89" spans="1:55">
@@ -19684,7 +19687,7 @@
       <c r="AC89" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="AD89" s="183"/>
+      <c r="AD89" s="171"/>
       <c r="AE89" s="107"/>
       <c r="AF89" s="44" t="s">
         <v>226</v>
@@ -19710,7 +19713,7 @@
       <c r="AO89" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="AP89" s="183"/>
+      <c r="AP89" s="171"/>
       <c r="AQ89" s="120" t="s">
         <v>228</v>
       </c>
@@ -19734,7 +19737,7 @@
       <c r="BA89" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BB89" s="177"/>
+      <c r="BB89" s="174"/>
       <c r="BC89" s="106"/>
     </row>
     <row r="90" spans="1:55">
@@ -19942,7 +19945,7 @@
       <c r="AC91" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AD91" s="185" t="s">
+      <c r="AD91" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AE91" s="108"/>
@@ -19974,7 +19977,7 @@
       <c r="AO91" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AP91" s="193" t="s">
+      <c r="AP91" s="175" t="s">
         <v>23</v>
       </c>
       <c r="AQ91" s="104"/>
@@ -19998,7 +20001,7 @@
       <c r="BA91" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="BB91" s="189" t="s">
+      <c r="BB91" s="178" t="s">
         <v>22</v>
       </c>
       <c r="BC91" s="118" t="s">
@@ -20091,7 +20094,7 @@
       <c r="AC92" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AD92" s="182"/>
+      <c r="AD92" s="170"/>
       <c r="AE92" s="106"/>
       <c r="AF92" s="43" t="s">
         <v>223</v>
@@ -20117,7 +20120,7 @@
       <c r="AO92" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AP92" s="194"/>
+      <c r="AP92" s="176"/>
       <c r="AQ92" s="102"/>
       <c r="AR92" s="43" t="s">
         <v>224</v>
@@ -20134,7 +20137,7 @@
       <c r="BA92" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB92" s="190"/>
+      <c r="BB92" s="179"/>
       <c r="BC92" s="119" t="s">
         <v>230</v>
       </c>
@@ -20227,7 +20230,7 @@
       <c r="AC93" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AD93" s="183"/>
+      <c r="AD93" s="171"/>
       <c r="AE93" s="107"/>
       <c r="AF93" s="44" t="s">
         <v>226</v>
@@ -20259,7 +20262,7 @@
       <c r="AO93" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AP93" s="195"/>
+      <c r="AP93" s="177"/>
       <c r="AQ93" s="103"/>
       <c r="AR93" s="44" t="s">
         <v>227</v>
@@ -20285,7 +20288,7 @@
       <c r="BA93" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="BB93" s="191"/>
+      <c r="BB93" s="180"/>
       <c r="BC93" s="136" t="s">
         <v>231</v>
       </c>
@@ -20372,7 +20375,7 @@
       <c r="AC94" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AD94" s="185" t="s">
+      <c r="AD94" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AE94" s="108"/>
@@ -20406,7 +20409,7 @@
       <c r="AO94" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AP94" s="193" t="s">
+      <c r="AP94" s="175" t="s">
         <v>23</v>
       </c>
       <c r="AQ94" s="104"/>
@@ -20430,7 +20433,7 @@
       <c r="BA94" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="BB94" s="184" t="s">
+      <c r="BB94" s="172" t="s">
         <v>24</v>
       </c>
       <c r="BC94" s="108"/>
@@ -20523,7 +20526,7 @@
       <c r="AC95" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AD95" s="182"/>
+      <c r="AD95" s="170"/>
       <c r="AE95" s="106"/>
       <c r="AF95" s="43" t="s">
         <v>223</v>
@@ -20553,7 +20556,7 @@
       <c r="AO95" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AP95" s="194"/>
+      <c r="AP95" s="176"/>
       <c r="AQ95" s="102"/>
       <c r="AR95" s="43" t="s">
         <v>224</v>
@@ -20570,7 +20573,7 @@
       <c r="BA95" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB95" s="176"/>
+      <c r="BB95" s="173"/>
       <c r="BC95" s="106"/>
     </row>
     <row r="96" spans="1:55">
@@ -20655,7 +20658,7 @@
       <c r="AC96" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="AD96" s="183"/>
+      <c r="AD96" s="171"/>
       <c r="AE96" s="107"/>
       <c r="AF96" s="44" t="s">
         <v>226</v>
@@ -20687,7 +20690,7 @@
       <c r="AO96" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AP96" s="195"/>
+      <c r="AP96" s="177"/>
       <c r="AQ96" s="103"/>
       <c r="AR96" s="44" t="s">
         <v>227</v>
@@ -20709,7 +20712,7 @@
       <c r="BA96" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BB96" s="177"/>
+      <c r="BB96" s="174"/>
       <c r="BC96" s="106"/>
     </row>
     <row r="97" spans="1:55">
@@ -21029,7 +21032,7 @@
       <c r="AC99" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="AD99" s="185" t="s">
+      <c r="AD99" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AE99" s="112" t="s">
@@ -21055,7 +21058,7 @@
       <c r="AO99" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="AP99" s="193" t="s">
+      <c r="AP99" s="175" t="s">
         <v>23</v>
       </c>
       <c r="AQ99" s="104"/>
@@ -21079,7 +21082,7 @@
       <c r="BA99" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="BB99" s="184" t="s">
+      <c r="BB99" s="172" t="s">
         <v>24</v>
       </c>
       <c r="BC99" s="108"/>
@@ -21154,7 +21157,7 @@
       <c r="AC100" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="AD100" s="182"/>
+      <c r="AD100" s="170"/>
       <c r="AE100" s="119" t="s">
         <v>240</v>
       </c>
@@ -21186,7 +21189,7 @@
       <c r="AO100" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AP100" s="194"/>
+      <c r="AP100" s="176"/>
       <c r="AQ100" s="102"/>
       <c r="AR100" s="43" t="s">
         <v>224</v>
@@ -21203,7 +21206,7 @@
       <c r="BA100" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB100" s="176"/>
+      <c r="BB100" s="173"/>
       <c r="BC100" s="106"/>
     </row>
     <row r="101" spans="1:55">
@@ -21284,7 +21287,7 @@
       <c r="AC101" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AD101" s="182"/>
+      <c r="AD101" s="170"/>
       <c r="AE101" s="119" t="s">
         <v>241</v>
       </c>
@@ -21318,7 +21321,7 @@
       <c r="AO101" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AP101" s="194"/>
+      <c r="AP101" s="176"/>
       <c r="AQ101" s="102"/>
       <c r="AR101" s="43" t="s">
         <v>224</v>
@@ -21335,7 +21338,7 @@
       <c r="BA101" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB101" s="176"/>
+      <c r="BB101" s="173"/>
       <c r="BC101" s="106"/>
     </row>
     <row r="102" spans="1:55">
@@ -21412,7 +21415,7 @@
       <c r="AC102" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AD102" s="182"/>
+      <c r="AD102" s="170"/>
       <c r="AE102" s="119" t="s">
         <v>241</v>
       </c>
@@ -21440,7 +21443,7 @@
       <c r="AO102" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AP102" s="194"/>
+      <c r="AP102" s="176"/>
       <c r="AQ102" s="102"/>
       <c r="AR102" s="43" t="s">
         <v>227</v>
@@ -21457,7 +21460,7 @@
       <c r="BA102" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB102" s="176"/>
+      <c r="BB102" s="173"/>
       <c r="BC102" s="106"/>
     </row>
     <row r="103" spans="1:55">
@@ -21532,7 +21535,7 @@
       <c r="AC103" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="AD103" s="183"/>
+      <c r="AD103" s="171"/>
       <c r="AE103" s="127" t="s">
         <v>239</v>
       </c>
@@ -21560,7 +21563,7 @@
       <c r="AO103" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="AP103" s="195"/>
+      <c r="AP103" s="177"/>
       <c r="AQ103" s="103"/>
       <c r="AR103" s="44" t="s">
         <v>224</v>
@@ -21582,7 +21585,7 @@
       <c r="BA103" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BB103" s="177"/>
+      <c r="BB103" s="174"/>
       <c r="BC103" s="106"/>
     </row>
     <row r="104" spans="1:55">
@@ -21783,7 +21786,7 @@
       <c r="AC105" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AD105" s="185" t="s">
+      <c r="AD105" s="169" t="s">
         <v>23</v>
       </c>
       <c r="AE105" s="108"/>
@@ -21815,7 +21818,7 @@
       <c r="AO105" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AP105" s="193" t="s">
+      <c r="AP105" s="175" t="s">
         <v>23</v>
       </c>
       <c r="AQ105" s="104"/>
@@ -21839,7 +21842,7 @@
       <c r="BA105" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="BB105" s="184" t="s">
+      <c r="BB105" s="172" t="s">
         <v>24</v>
       </c>
       <c r="BC105" s="108"/>
@@ -21924,7 +21927,7 @@
       <c r="AC106" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AD106" s="182"/>
+      <c r="AD106" s="170"/>
       <c r="AE106" s="106"/>
       <c r="AF106" s="43" t="s">
         <v>226</v>
@@ -21954,7 +21957,7 @@
       <c r="AO106" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AP106" s="194"/>
+      <c r="AP106" s="176"/>
       <c r="AQ106" s="102"/>
       <c r="AR106" s="43" t="s">
         <v>227</v>
@@ -21971,7 +21974,7 @@
       <c r="BA106" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB106" s="176"/>
+      <c r="BB106" s="173"/>
       <c r="BC106" s="106"/>
     </row>
     <row r="107" spans="1:55">
@@ -22054,7 +22057,7 @@
       <c r="AC107" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AD107" s="182"/>
+      <c r="AD107" s="170"/>
       <c r="AE107" s="106"/>
       <c r="AF107" s="43" t="s">
         <v>223</v>
@@ -22086,7 +22089,7 @@
       <c r="AO107" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AP107" s="194"/>
+      <c r="AP107" s="176"/>
       <c r="AQ107" s="102"/>
       <c r="AR107" s="43" t="s">
         <v>224</v>
@@ -22103,7 +22106,7 @@
       <c r="BA107" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB107" s="176"/>
+      <c r="BB107" s="173"/>
       <c r="BC107" s="106"/>
     </row>
     <row r="108" spans="1:55">
@@ -22186,7 +22189,7 @@
       <c r="AC108" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AD108" s="182"/>
+      <c r="AD108" s="170"/>
       <c r="AE108" s="106"/>
       <c r="AF108" s="43" t="s">
         <v>226</v>
@@ -22212,7 +22215,7 @@
       <c r="AO108" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AP108" s="194"/>
+      <c r="AP108" s="176"/>
       <c r="AQ108" s="102"/>
       <c r="AR108" s="43" t="s">
         <v>227</v>
@@ -22229,7 +22232,7 @@
       <c r="BA108" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB108" s="176"/>
+      <c r="BB108" s="173"/>
       <c r="BC108" s="106"/>
     </row>
     <row r="109" spans="1:55">
@@ -22314,7 +22317,7 @@
       <c r="AC109" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AD109" s="183"/>
+      <c r="AD109" s="171"/>
       <c r="AE109" s="107"/>
       <c r="AF109" s="44" t="s">
         <v>226</v>
@@ -22344,7 +22347,7 @@
       <c r="AO109" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="AP109" s="195"/>
+      <c r="AP109" s="177"/>
       <c r="AQ109" s="103"/>
       <c r="AR109" s="44" t="s">
         <v>227</v>
@@ -22366,7 +22369,7 @@
       <c r="BA109" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BB109" s="177"/>
+      <c r="BB109" s="174"/>
       <c r="BC109" s="106"/>
     </row>
     <row r="110" spans="1:55">
@@ -22569,7 +22572,7 @@
       <c r="AC111" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="AD111" s="184" t="s">
+      <c r="AD111" s="172" t="s">
         <v>24</v>
       </c>
       <c r="AE111" s="108"/>
@@ -22603,7 +22606,7 @@
       <c r="AO111" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AP111" s="193" t="s">
+      <c r="AP111" s="175" t="s">
         <v>23</v>
       </c>
       <c r="AQ111" s="104"/>
@@ -22627,7 +22630,7 @@
       <c r="BA111" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="BB111" s="184" t="s">
+      <c r="BB111" s="172" t="s">
         <v>24</v>
       </c>
       <c r="BC111" s="108"/>
@@ -22708,7 +22711,7 @@
       <c r="AC112" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="AD112" s="176"/>
+      <c r="AD112" s="173"/>
       <c r="AE112" s="106"/>
       <c r="AF112" s="43" t="s">
         <v>223</v>
@@ -22730,7 +22733,7 @@
       <c r="AO112" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="AP112" s="194"/>
+      <c r="AP112" s="176"/>
       <c r="AQ112" s="102"/>
       <c r="AR112" s="43" t="s">
         <v>224</v>
@@ -22747,7 +22750,7 @@
       <c r="BA112" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB112" s="176"/>
+      <c r="BB112" s="173"/>
       <c r="BC112" s="106"/>
     </row>
     <row r="113" spans="1:55">
@@ -22826,7 +22829,7 @@
       <c r="AC113" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="AD113" s="176"/>
+      <c r="AD113" s="173"/>
       <c r="AE113" s="106"/>
       <c r="AF113" s="43" t="s">
         <v>223</v>
@@ -22856,7 +22859,7 @@
       <c r="AO113" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AP113" s="194"/>
+      <c r="AP113" s="176"/>
       <c r="AQ113" s="102"/>
       <c r="AR113" s="43" t="s">
         <v>224</v>
@@ -22873,7 +22876,7 @@
       <c r="BA113" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BB113" s="176"/>
+      <c r="BB113" s="173"/>
       <c r="BC113" s="106"/>
     </row>
     <row r="114" spans="1:55">
@@ -22952,7 +22955,7 @@
       <c r="AC114" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="AD114" s="177"/>
+      <c r="AD114" s="174"/>
       <c r="AE114" s="107"/>
       <c r="AF114" s="44" t="s">
         <v>226</v>
@@ -22978,7 +22981,7 @@
       <c r="AO114" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="AP114" s="195"/>
+      <c r="AP114" s="177"/>
       <c r="AQ114" s="103"/>
       <c r="AR114" s="44" t="s">
         <v>227</v>
@@ -23000,7 +23003,7 @@
       <c r="BA114" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BB114" s="177"/>
+      <c r="BB114" s="174"/>
       <c r="BC114" s="106"/>
     </row>
     <row r="115" spans="1:55">
@@ -24044,6 +24047,90 @@
     <sortCondition ref="B3:B114"/>
   </sortState>
   <mergeCells count="100">
+    <mergeCell ref="N1:S1"/>
+    <mergeCell ref="T1:AC1"/>
+    <mergeCell ref="AF1:AO1"/>
+    <mergeCell ref="AR1:BA1"/>
+    <mergeCell ref="BB3:BB5"/>
+    <mergeCell ref="AD3:AD5"/>
+    <mergeCell ref="AP3:AP5"/>
+    <mergeCell ref="BB6:BB8"/>
+    <mergeCell ref="AP6:AP8"/>
+    <mergeCell ref="AD6:AD8"/>
+    <mergeCell ref="BB9:BB11"/>
+    <mergeCell ref="AP9:AP11"/>
+    <mergeCell ref="AD9:AD11"/>
+    <mergeCell ref="BB13:BB15"/>
+    <mergeCell ref="AP13:AP15"/>
+    <mergeCell ref="AD13:AD15"/>
+    <mergeCell ref="BB16:BB18"/>
+    <mergeCell ref="AP16:AP18"/>
+    <mergeCell ref="AD16:AD18"/>
+    <mergeCell ref="BB19:BB21"/>
+    <mergeCell ref="AP19:AP21"/>
+    <mergeCell ref="AD19:AD21"/>
+    <mergeCell ref="BB22:BB24"/>
+    <mergeCell ref="AD22:AD24"/>
+    <mergeCell ref="AP22:AP24"/>
+    <mergeCell ref="BB25:BB27"/>
+    <mergeCell ref="AP25:AP27"/>
+    <mergeCell ref="AD25:AD27"/>
+    <mergeCell ref="BB29:BB31"/>
+    <mergeCell ref="AP29:AP31"/>
+    <mergeCell ref="AD29:AD31"/>
+    <mergeCell ref="BB33:BB35"/>
+    <mergeCell ref="AP33:AP35"/>
+    <mergeCell ref="AD33:AD35"/>
+    <mergeCell ref="BB36:BB38"/>
+    <mergeCell ref="BB39:BB41"/>
+    <mergeCell ref="AD36:AD38"/>
+    <mergeCell ref="AD39:AD41"/>
+    <mergeCell ref="AP36:AP38"/>
+    <mergeCell ref="AP39:AP41"/>
+    <mergeCell ref="AD42:AD44"/>
+    <mergeCell ref="AD45:AD47"/>
+    <mergeCell ref="AD48:AD50"/>
+    <mergeCell ref="AD51:AD53"/>
+    <mergeCell ref="AD54:AD56"/>
+    <mergeCell ref="AD57:AD59"/>
+    <mergeCell ref="AD60:AD62"/>
+    <mergeCell ref="AD63:AD65"/>
+    <mergeCell ref="AD68:AD70"/>
+    <mergeCell ref="AD71:AD73"/>
+    <mergeCell ref="AP42:AP44"/>
+    <mergeCell ref="AP45:AP47"/>
+    <mergeCell ref="AP48:AP50"/>
+    <mergeCell ref="AP51:AP53"/>
+    <mergeCell ref="AP57:AP59"/>
+    <mergeCell ref="AP60:AP62"/>
+    <mergeCell ref="AP63:AP65"/>
+    <mergeCell ref="AP68:AP70"/>
+    <mergeCell ref="AP71:AP73"/>
+    <mergeCell ref="AP75:AP77"/>
+    <mergeCell ref="BB42:BB44"/>
+    <mergeCell ref="BB45:BB47"/>
+    <mergeCell ref="BB48:BB50"/>
+    <mergeCell ref="BB51:BB53"/>
+    <mergeCell ref="BB54:BB56"/>
+    <mergeCell ref="BB57:BB59"/>
+    <mergeCell ref="BB60:BB62"/>
+    <mergeCell ref="BB71:BB73"/>
+    <mergeCell ref="BB63:BB65"/>
+    <mergeCell ref="BB68:BB70"/>
+    <mergeCell ref="BB111:BB114"/>
+    <mergeCell ref="BB99:BB103"/>
+    <mergeCell ref="BB105:BB109"/>
+    <mergeCell ref="BB75:BB77"/>
+    <mergeCell ref="BB91:BB93"/>
+    <mergeCell ref="BB78:BB80"/>
+    <mergeCell ref="BB81:BB83"/>
+    <mergeCell ref="BB84:BB86"/>
+    <mergeCell ref="BB87:BB89"/>
+    <mergeCell ref="AP81:AP83"/>
+    <mergeCell ref="AP84:AP86"/>
+    <mergeCell ref="AP87:AP89"/>
+    <mergeCell ref="AP91:AP93"/>
+    <mergeCell ref="BB94:BB96"/>
     <mergeCell ref="AD75:AD77"/>
     <mergeCell ref="AD87:AD89"/>
     <mergeCell ref="AP54:AP56"/>
@@ -24060,90 +24147,6 @@
     <mergeCell ref="AD91:AD93"/>
     <mergeCell ref="AD94:AD96"/>
     <mergeCell ref="AP78:AP80"/>
-    <mergeCell ref="AP81:AP83"/>
-    <mergeCell ref="AP84:AP86"/>
-    <mergeCell ref="AP87:AP89"/>
-    <mergeCell ref="AP91:AP93"/>
-    <mergeCell ref="BB94:BB96"/>
-    <mergeCell ref="BB111:BB114"/>
-    <mergeCell ref="BB99:BB103"/>
-    <mergeCell ref="BB105:BB109"/>
-    <mergeCell ref="BB75:BB77"/>
-    <mergeCell ref="BB91:BB93"/>
-    <mergeCell ref="BB78:BB80"/>
-    <mergeCell ref="BB81:BB83"/>
-    <mergeCell ref="BB84:BB86"/>
-    <mergeCell ref="BB87:BB89"/>
-    <mergeCell ref="BB57:BB59"/>
-    <mergeCell ref="BB60:BB62"/>
-    <mergeCell ref="BB71:BB73"/>
-    <mergeCell ref="BB63:BB65"/>
-    <mergeCell ref="BB68:BB70"/>
-    <mergeCell ref="BB42:BB44"/>
-    <mergeCell ref="BB45:BB47"/>
-    <mergeCell ref="BB48:BB50"/>
-    <mergeCell ref="BB51:BB53"/>
-    <mergeCell ref="BB54:BB56"/>
-    <mergeCell ref="AP60:AP62"/>
-    <mergeCell ref="AP63:AP65"/>
-    <mergeCell ref="AP68:AP70"/>
-    <mergeCell ref="AP71:AP73"/>
-    <mergeCell ref="AP75:AP77"/>
-    <mergeCell ref="AP42:AP44"/>
-    <mergeCell ref="AP45:AP47"/>
-    <mergeCell ref="AP48:AP50"/>
-    <mergeCell ref="AP51:AP53"/>
-    <mergeCell ref="AP57:AP59"/>
-    <mergeCell ref="AD57:AD59"/>
-    <mergeCell ref="AD60:AD62"/>
-    <mergeCell ref="AD63:AD65"/>
-    <mergeCell ref="AD68:AD70"/>
-    <mergeCell ref="AD71:AD73"/>
-    <mergeCell ref="AD42:AD44"/>
-    <mergeCell ref="AD45:AD47"/>
-    <mergeCell ref="AD48:AD50"/>
-    <mergeCell ref="AD51:AD53"/>
-    <mergeCell ref="AD54:AD56"/>
-    <mergeCell ref="BB33:BB35"/>
-    <mergeCell ref="AP33:AP35"/>
-    <mergeCell ref="AD33:AD35"/>
-    <mergeCell ref="BB36:BB38"/>
-    <mergeCell ref="BB39:BB41"/>
-    <mergeCell ref="AD36:AD38"/>
-    <mergeCell ref="AD39:AD41"/>
-    <mergeCell ref="AP36:AP38"/>
-    <mergeCell ref="AP39:AP41"/>
-    <mergeCell ref="BB25:BB27"/>
-    <mergeCell ref="AP25:AP27"/>
-    <mergeCell ref="AD25:AD27"/>
-    <mergeCell ref="BB29:BB31"/>
-    <mergeCell ref="AP29:AP31"/>
-    <mergeCell ref="AD29:AD31"/>
-    <mergeCell ref="BB19:BB21"/>
-    <mergeCell ref="AP19:AP21"/>
-    <mergeCell ref="AD19:AD21"/>
-    <mergeCell ref="BB22:BB24"/>
-    <mergeCell ref="AD22:AD24"/>
-    <mergeCell ref="AP22:AP24"/>
-    <mergeCell ref="BB13:BB15"/>
-    <mergeCell ref="AP13:AP15"/>
-    <mergeCell ref="AD13:AD15"/>
-    <mergeCell ref="BB16:BB18"/>
-    <mergeCell ref="AP16:AP18"/>
-    <mergeCell ref="AD16:AD18"/>
-    <mergeCell ref="BB6:BB8"/>
-    <mergeCell ref="AP6:AP8"/>
-    <mergeCell ref="AD6:AD8"/>
-    <mergeCell ref="BB9:BB11"/>
-    <mergeCell ref="AP9:AP11"/>
-    <mergeCell ref="AD9:AD11"/>
-    <mergeCell ref="N1:S1"/>
-    <mergeCell ref="T1:AC1"/>
-    <mergeCell ref="AF1:AO1"/>
-    <mergeCell ref="AR1:BA1"/>
-    <mergeCell ref="BB3:BB5"/>
-    <mergeCell ref="AD3:AD5"/>
-    <mergeCell ref="AP3:AP5"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -24176,15 +24179,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004D6AAE0340A76546AEC815625A74F0D3" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="37ce713dd9ea8860b41d5fa2c11a466e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c1447db-1895-44e3-90e5-6612ffa61a2c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2879ffd319974e0a205d8716a0fb19a4" ns2:_="">
     <xsd:import namespace="9c1447db-1895-44e3-90e5-6612ffa61a2c"/>
@@ -24362,14 +24356,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD4F6C4D-B26B-4A68-B677-6F8071D5552D}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6766F99-0218-4744-A129-24116F201A28}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6A0DCA8-7B8B-410B-9569-33EA049CF5D6}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6A0DCA8-7B8B-410B-9569-33EA049CF5D6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6766F99-0218-4744-A129-24116F201A28}"/>
 </file>
</xml_diff>